<commit_message>
added sources tooltip to each assistant message
</commit_message>
<xml_diff>
--- a/query/legal_questions_answers_english.xlsx
+++ b/query/legal_questions_answers_english.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,1749 +473,2004 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>How can I apply for a temporary residence permit in Lower Silesia?</t>
+          <t>What rights do I have as a foreign worker in Poland?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://przybysz.duw.pl/cudzoziemcy-pobyt/zezwolenia-na-pobyt-czasowy/pobyt-czasowy-i-praca/</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00214</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Who makes the request?
-When should I/we submit the application?
-How do I submit an application?
-What documents do I need to submit?
-What are the fees?</t>
+          <t>Regardless of whether you employ a foreigner in Poland or delegate him/her to provide services in the territory of Poland, as the entity entrusting the work you must ensure employment conditions that are in accordance with Polish regulations. If a foreigner is employed/delegated to Poland and performs work on the basis of an employment contract, the rule is that his employment conditions cannot be less favorable than those guaranteed by Polish labor laws . norms and dimensions of working time and periods of daily and weekly rest,</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://przybysz.duw.pl/cudzoziemcy-pobyt/zezwolenia-na-pobyt-czasowy/zezwolenie-na-pobyt-czasowy-w-celu-wykonywania-pracy-przez-cudzoziemca-w-ramach-przeniesienie-wewnatrz-przedsiebiorstwa/</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00198</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Who makes the request?
-When should I/we submit the application?
-How do I submit an application?
-What documents do I need to submit?
-What are the fees?</t>
+          <t>Obligations of an employer posting an employee from a third country An employer posting from a third country shall comply with: all regulations related to the posting of an employee in the territory of Poland</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://pro4work.pl/zlozenie-wniosku-na-karte-pobytu-krok-po-kroku/</t>
+          <t>https://www.biznes.gov.pl/pl/portal/004330</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Applying for a residence card at the Lower Silesian Provincial Office in Wroclaw for legalization of stay and work is currently a big problem for a Foreigner. At the moment, the only way to apply for a residence card at the Lower Silesian Provincial Office is to register through the "DOLNOŚLĄSKIE VISIT RESERVATION SYSTEM".
-Foreigners can no longer apply for a residence card by going to the Office and taking the appropriate ticket from a ticket machine, as was the case a few months ago. Remember that the application to legalize the stay is submitted during the foreigner's legal stay in Poland.
-The first step to start the procedure for applying for a temporary residence decision (residence card) is to register a user account on the website:
-https://rezerwacje.duw.pl/reservations/pol/login
-</t>
+          <t>A foreigner who is a citizen of a country outside the European Union , the European Economic Area or Switzerland may legally work in Poland, provided that he or she meets the following conditions together: legally resides in the territory of Poland, i.e. has the appropriate residence documents if he or she is not exempt from the obligation to have a work permit, then: he obtains a temporary residence and work permit or the employer obtains for him a work permit, a seasonal work permit or submits a statement on entrusting work to a foreigner his residence documents allow him to perform work his work is performed under the conditions and in the position specified in the work permit, statement on entrusting work or temporary residence and work permit .</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>What are the requirements for permanent residency in Lower Silesia?</t>
+          <t>What services are available at the office for foreigners?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://przybysz.duw.pl/cudzoziemcy-pobyt/zezwolenia-na-pobyt-staly/</t>
+          <t>https://www.gov.pl/web/udsc/rodzaje-przyznawanej-pomocy</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Who makes the request?
-When should I/we submit the application?
-How do I submit an application?
-What documents do I need to submit?
-What are the fees?</t>
+          <t>reimbursement of the cost of travel by public transport in certain cases, i.e. related to the refugee status procedure, to attend medical examinations or immunizations or in other justified cases; permanent cash assistance for the purchase of personal hygiene products - PLN 20 per month and the so-called "pocket money" - PLN 50 per month; provision of one-time cash assistance for the purchase of clothing and footwear - PLN 140;</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://firmadlakazdego.pl/jak-uzyskac-karte-stalego-pobytu-w-polsce/</t>
+          <t>https://www.gov.pl/web/udsc/zadania-realizowane-przez-urzad-do-spraw-cudzoziemcow</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>October 17, 2024
-Process for obtaining a permanent residence card
-Requirements for a permanent residence card
-Documents needed for permanent residence card</t>
+          <t>The Head of the Office for Foreigners, as a central body of government administration, performs the following tasks: considers appeals against the decisions of governors in matters of legalization of residence - residence permits for foreigners, visas and invitations, registration of residence and the right of permanent residence of citizens of the European Union and their family members, and controls governors in this regard; conducts visa consultations and exchanges data between member states on visas;</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://migrant.wsc.mazowieckie.pl/pl/procedury/wydanie-karty-pobytu-na-wniosek</t>
+          <t>https://www.katowice.uw.gov.pl/usluga/cudzoziemcy</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Go to main menu
-Skip to content
-Availability
-Home page
-Procedures</t>
+          <t>"ŚLĄSKIE FOR FOREIGNERS". Project FAMI.02.01-IZ.00-0002/24 co-financed by the Asylum, Migration and Integration Fund for 2021-2027 Temporary stay, permanent stay, long-term resident of the EU, visas, cash benefits for the holders of the Card of the Pole MODE OF APPLICATION - INTERNET RESERVATION</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Can I work in Lower Silesia on a student visa?</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
+          <t>What are the consequences of overstaying a visa in Polsky?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/attachment/c4067bab-e664-4072-8be5-6c90367ab4e3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Obligation of a foreigner to return - Chapter 2 - Laws Control of legality of stay of foreigners in the territory of ... Informing the foreigner about the rules and procedure ...</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://pckp.pl/baza-wiedzy/jak-legalnie-zatrudnic-cudzoziemca-bedacego-studentem-polskiej-uczelni/</t>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/ruch-cudzoziemcow-16868620</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Consent
-Details
-[#IABV2SETTINGS#]
-About cookies
-Essential 12 Essential cookies contribute to the usability of the website by enabling basic functions such as site navigation and access to secure areas of the website. A website cannot function properly without these cookies.Cookiebot1Learn more about this providerCookieConsentStores the user's cookie consent state for the current domainMaximum retention period: 1 yearName: HTT cookiePGoogle4Learn more about this providerSome of the data collected by this provider is used to personalize and measure the effectiveness of advertising.test_cookieUsed to check if the user's browser supports cookies.Maximum retention period: 1 dayName: HTTPar_debugChecks whether a technical debugger-cookie is present. Maximum retention period: 3 monthsName: HTTPrc cookie::aThis cookie is used to distinguish between humans and bots. This is beneficial for the website, in order to make valid reports on the use of their website.Maximum retention period: PermanentName: Local HTMLrc storage::cThis cookie is used to distinguish between humans and bots. Maximum retention period: SessionalName: Local HTMLLinkedIn2Learn more about this providerbcookieUsed in order to detect spam and improve the website's security. Maximum retention period: 1 yearName: HTTPli_gcStores the user's cookie consent state for the current domainMaximum retention period: 180 daysName: HTTPSales cookie Manago1Learn more about this providerSERVERIDThis cookie is used to assign the visitor to a specific server - this function is necessary for the functionality of the website.Maximum retention period: SessionName: HTTP cookieVimeo2Learn more about this provider__cf_bmThis cookie is used to distinguish between humans and bots. This is beneficial for the website, in order to make valid reports on the use of their website.Maximum retention period: 1 dayName: HTTP_cfuvidThis cookie is a part of the services provided by Cloudflare - Including load-balancing, delivery of website content and serving DNS connection for website operators. Maximum retention period: SessionName: HTTPpckp.pl2storeApiNonceNecessary for the shopping cart functionality on the website.Maximum retention period: PersistentName: Local HTML storagewpEmojiSettingsSupportsThis cookie is part of a bundle of cookies which serve the purpose of content delivery and presentation. The cookies keep the correct state of font, blog/picture sliders, color themes and other website settings.Maximum retention period: SessionalName: Local HTML storage.</t>
+          <t>REGULATION OF THE MINISTER OF INTERNAL AFFAIRS of November 8, 1929 on the movement of foreigners, issued as to §§ 1, 2, 3, 4, 5, 9, 10, 11, 13, 14, 15, 16, 17, 20, 21, 24, 38, 40, 41, 42, 43, 44, 47, 52 and 53 in agreement with the Minister of Foreign Affairs. A residence visa may authorize multiple crossings of the borders of the Republic. On the other hand, a residence visa until further notice is granted by the consular post when the purpose of the stay is of such a nature that the time required to achieve it cannot be determined even approximately.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://klubjagiellonski.pl/2025/03/18/w-polsce-jest-az-107-tys-studentow-z-zagranicy-to-szansa-czy-moze-zagrozenie/</t>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/cudzoziemcy-18053962/dz-8-roz-2</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>The number of foreign students in Poland is growing - in the past academic year there were already more than 107,000 of them studying in our country. They study equally at private and public universities, and the majors they most often choose are management, information technology and medical faculties. Is the increase in the number of foreigners studying at our universities a positive development, and can we as a society benefit from it?
-A review of the annual report Foreign Students in Poland by the Study in Poland Foundation, which cooperates with Perspektywy magazine, leaves no doubt: the number of foreign students in Poland is growing rapidly. While at the beginning of this century there were just over 6,500 foreigners studying in our country, by the 2023/2024 academic year this number will exceed 107,000.
-The issue of foreign students at Polish universities came under the lens of public opinion following the announcement of the migration strategy for 2025-2030 by Donald Tusk's government last fall. The document announces the fight against uncontrolled migration from outside OECD countries, which, in perspective, could also ricochet on those who would like to come to Poland to pursue their academic passions.
-A vein of gold for universities?</t>
+          <t>Chapter 2 - Obligation of a foreigner to return - Foreigners. - has become final, and if a decision has been issued by a higher level authority - from the date on which the decision has been delivered to the foreigner; The authority conducting the proceedings on the foreigner's obligation to return shall instruct the foreigner on the possibility of filing an application for international protection.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>How long can I stay in Lower Silesia after my visa expires?</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+          <t>How to report the birth of a child in Poland?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/gov/zglos-urodzenie-dziecka</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>If you have a baby, you need to report it to the appropriate registry office . The head of the office will register the birth of the child, give you its PESEL number and register it. Find out how to report the birth of a child - online or in the office. If you want to report the birth of a child online - you need a trusted profile or an e-card. They allow you to confirm your identity. Check out how to set up a trusted profile or how to use an e-card.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/cyfryzacja/co-jest-potrzebne-by-zglosic-narodziny-dziecka-imie-i-internet</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>What is needed to report the birth of a child? A name and... the Internet! Johnny, Bozydar, Grześ, Kociemir - choosing a name for a child is not always easy. It is very simple, on the other hand, to report the birth of a new family member. The easiest and fastest way to do this is via the Internet - on GOV.pl. Starting today on TV and the Internet, you can watch our latest spot, in which we encourage you to take advantage of this opportunity. This is another installment of our "e-Poland can!" campaign.</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://archiwum.mswia.gov.pl/pl/sprawy-obywatelskie/rejestracja-stanu-cywi/12970,Jak-zarejestrowac-urodzenie-malzenstwo-zgon.html</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Forms of marriage Marriage before the head of the registry office Marriage outside the registry office Before a clergyman - religious marriage with civil-legal effects before a consul Marriage outside the registry office Marriage before the head of the registry office Marriage outside the registry office Before a clergyman - religious marriage with civil-legal effects before a consul</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>What are the consequences of overstaying a visa in Lower Silesia?</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+          <t>How do I apply for a temporary residence permit in Poland?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00210</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>The procedure for obtaining a temporary residence and work permit, i.e. a unified permit, is advantageous because all the formalities legalizing a foreigner's stay and employment take place under a single administrative procedure - the foreigner does not have to apply separately for a residence permit , and the employer - for a work permit. The provincial governor, who has granted a uniform permit for temporary residence and work in the territory of Poland, issues a residence card to the foreigner ex officio. The residence card, during the period in which it is valid, confirms the identity of the foreigner and entitles him, together with a travel document, to repeatedly cross the border without the need to obtain a visa.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://biznes.gov.pl/pl/portal/ou1613</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Obtain a Temporary Residence Permit for the Purpose of Performing Highly Qualified Work Are you a foreigner, have high professional qualifications and want to work in Poland? Find out how to obtain a temporary residence permit in Poland to perform highly qualified work. What you should know and who can benefit from the service</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/uw-warminsko-mazurski/cudzoziemcy---zezwolenia-na-pobyt-czasowy-na-terytorium-rp</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Detailed information can be found on the website of the Office for Foreigners in the Case Service Module at the following link: https://www.mos.cudzoziemcy.gov.pl/potrzebuje-informacji/pobyt-czas https://mos.cudzoziemcy.gov.pl/potrzebuje-informacji/szczegolne-okol</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Do I need a work permit in Lower Silesia?</t>
+          <t>Can I work in Poland on a student visa?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://przybysz.duw.pl/cudzoziemcy-praca/zezwolenie-na-prace/</t>
+          <t>https://zielonalinia.gov.pl/-/student-cudzoziemiec-a-obowiazek-posiadania-zezwolenia-na-prace</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">What documents do I need to submit (by permit type)?
-How do I submit an application?
-What are the fees?
-What do I need to know?
-</t>
+          <t>The issue of exemption from the requirement for a third-country foreigner to have a work permit is regulated by the provisions of the Employment Promotion and Labor Market Institutions Act and the Ordinance of the Minister of Labor and Social Policy on cases in which entrusting work to a foreigner in the territory of the Republic of Poland is permissible without the need to obtain a work permit. We read about students in § 1 item 10 of the above-mentioned regulation. According to this provision, entrusting a foreigner with work in the territory of the Republic of Poland without the need to obtain a work permit is permissible in the case of foreigners who are students of full-time studies held in the Republic of Poland or participants in full-time doctoral studies held in the Republic of Poland. Read also: Basic obligation of an employer who wants to hire a foreigner</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://przybysz.duw.pl/cudzoziemcy-pobyt/zezwolenia-na-pobyt-czasowy/pobyt-czasowy-i-praca/</t>
+          <t>https://www.biznes.gov.pl/pl/portal/004330</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Who makes the request?
-When should I/we submit the application?
-How do I submit an application?
-What documents do I need to submit?
-What are the fees?</t>
+          <t>A foreigner who is a citizen of a country outside the European Union , the European Economic Area or Switzerland may legally work in Poland, provided that he or she meets the following conditions together: legally resides in the territory of Poland, i.e. has the appropriate residence documents if he or she is not exempt from the obligation to have a work permit, then: he obtains a temporary residence and work permit or the employer obtains for him a work permit, a seasonal work permit or submits a statement on entrusting work to a foreigner his residence documents allow him to perform work his work is performed under the conditions and in the position specified in the work permit, statement on entrusting work or temporary residence and work permit .</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://askor.waw.pl/zezwolenie-na-prace-wroclaw/</t>
+          <t>https://www.biznes.gov.pl/pl/portal/004330#1</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Work permit Wrocław - who is affected ?
-If you employ foreigners from outside the EU, EEA and Switzerland, you will need a work permit for your employees.  The work permit is issued by the relevant provincial governor. Accordingly, an application for a work permit is submitted by the employer to the provincial office. If the registered office or place of residence of the employer is in the territory of the Lower Silesian province, then without a doubt the application for a permit can be submitted to the Lower Silesian Provincial Office. The application for a type A work permit concerns a foreigner performing work in the territory of Poland on the basis of a contract with an entity. The permit applies to work performed for that particular employer. It is important to remember that it is not valid for employment with another employer. At the same time, when hiring a foreigner, you need to know what kind of work permit you need.
-Check out the types of work permits &gt;&gt;
-The application for a work permit for a foreigner should be submitted through the Lower Silesian Provincial Office in Wroclaw. You can apply for a Wroclaw work permit in person or order it through an online service.
-Work permits for foreigners || order &gt;&gt;.</t>
+          <t>A foreigner who is a citizen of a country outside the European Union , the European Economic Area or Switzerland may legally work in Poland, provided that he or she meets the following conditions together: legally resides in the territory of Poland, that is, has the appropriate residence documents if he or she is not exempted from the obligation to have a work permit, then: he obtains a temporary residence and work permit or the employer obtains for him a work permit, a seasonal work permit or submits a statement on entrusting work to a foreigner his residence documents allow him to perform work his work is performed on the conditions and position that have been specified in the work permit, statement on entrusting work or temporary residence and work permit .</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>How can I get a work permit as a non-EU citizen in Lower Silesia?</t>
+          <t>Can a foreigner open a business in Polish?</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://migrant.wsc.mazowieckie.pl/pl/faq/wydaniewymiana-karty-pobytu</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00806</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Go to main menu
-Skip to content
-Availability
-Home page
-temporary residence permit for the purpose of family reunification, and on the date of application for this permit you were outside the Republic of Poland,</t>
+          <t>Who can do business in Poland Citizens of the European Union member states and the European Economic Area who want to do business in Poland can: set up their own sole proprietorship or any commercial company</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://infoopt.pl/ogolne-zasady-zatrudniania-cudzoziemcow-w-polsce/</t>
+          <t>https://www.biznes.gov.pl/pl/portal/0613</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>The rules for the stay of third-country nationals in the territory of the Republic of Poland are set forth in the Act of December 12, 2013 on foreigners, while the rules for their employment are set forth in the provisions of the Act of April 20, 2004 on employment promotion and labor market institutions.
-reside legally in the territory of the Republic of Poland, i.e. have one of the following documents, i.e.:
-A valid visa*
-A residence permit,
-A stamp in your passport confirming that you have applied for temporary residency,</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+          <t>Who can do business in Poland Polish regulations provide for a great deal of freedom in business, which means that in most cases you can set up a company and run it in the form you choose. Read when you need to meet additional conditions. Find out if a company can be opened by a foreigner, a minor or a pensioner. Foreigner's company Setting up a sole proprietorship Polish legislation provides for a great deal of freedom in business, which means that in most cases you can set up a company and run it in the form of your choice. Read when you need to meet additional conditions. Find out if a foreigner, a minor or a pensioner can open a company. How to delegate employees to Poland in the framework of the provision of services Find out what delegation in the framework of the provision of services consists of, what are the rules and obligations of delegating employers, when an employee is a delegated employee. Foreigner's company Delegation Obligations of the employer Employment of an employee</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/001466</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>A citizen of Ukraine who resides in Poland legally and has a PESEL number may establish a business on the same terms as a Polish citizen in any form. a sole proprietorship - i.e., a business activity of a natural person - and register it with the CEIDG a partnership or a corporation - including a general partnership and a partnership - and register it with the National Court Register.</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>What rights do I have as a foreign worker in Lower Silesia?</t>
+          <t>How to extend a visa in Poland?</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://hrappka.pl/blog/cudzoziemcy/pit-11-czy-ift-1r-jak-rozliczyc-cudzoziemca</t>
+          <t>https://migrant.poznan.uw.gov.pl/pl/procedury/przedluzenie-wizy-krajowej</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>January is an important month for employers. They are obliged to provide the Tax Office with the relevant tax returns. When employing people from Poland, the matter is obvious - the employer issues a PIT-11. However, doubts arise when employing foreigners. How to account for individuals who do not reside in Poland? What annual declaration should be issued to a foreigner employed on the basis of a statement of entrustment of work to a foreigner or on the basis of a work permit? We answer in the article.
-&gt;&gt; Test your HR and payroll system for free
-Issues raised in the article:
-The first and most important step is to determine the tax residency of a foreigner. It determines which country should be the first to pay tax on income.
-For tax purposes, a Polish tax resident is a person who lives in Poland for more than 183 days a year, or a person who resides here for a shorter period, but has a center of personal, life and economic interests in Poland. Such a person is subject to so-called unlimited tax liability.</t>
+          <t>You apply for an extension of your national visa no later than the last day of the validity of the visa you have. If you submit your application on time and there are no formal deficiencies in it, or if you correct the formal deficiencies within the period we indicate, your stay will be legal from the date of your application until the date on which the decision on this matter becomes final. Before submitting your application, read our guidance on how to fill out application forms</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://hrappka.pl/blog/pit-2-dla-cudzoziemca-co-warto-wiedziec</t>
+          <t>https://www.katowice.uw.gov.pl/usluga/cudzoziemcy/przedluzenie-wizy-schengen-lub-wizy-krajowej</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Author
-Andrew Tkaczuk
-Legalization Specialist
-foreigners</t>
+          <t>I Who can apply for visa extension If you are a foreigner residing in the territory of the Republic of Poland, you can apply for extension of the validity period of a national visa issued by a Polish authority or the length of stay covered by this visa. If you are a foreigner residing on the territory of the Republic of Poland, you may apply for an extension of the validity period of a Schengen visa issued by a Polish authority or an authority of another Schengen area country that is also valid on the territory of Poland or the length of stay covered by this visa. If you are a foreigner residing in the territory of the Republic of Poland, you may apply for an extension of the validity period of a national visa issued by a Polish authority or the length of stay covered by this visa. If you are a foreigner residing in the territory of the Republic of Poland, you may apply for an extension of the validity period of a Schengen visa issued by a Polish authority or an authority of another Schengen area country that is also valid in the territory of Poland or the length of stay covered by this visa. II Documents The foreigner applying for extension of Schengen visa or national visa is obliged to: submit a completed application form for extension of Schengen visa or national visa , present a valid travel document, justify the application, and attach to the application: 1. A current photograph - undamaged, color, 35 x 45 mm, taken within the last 6 months on a uniform bright background, having good sharpness and showing clearly the eyes and face from the top of the head to the upper part of the shoulders, so that the face occupies 70-80% of the photograph; the photograph should depict a person without headgear and glasses with dark glasses, looking straight ahead with open eyes, uncovered hair, with a natural expression on the face and closed mouth; ✸ Attention! A foreigner who wears headgear in accordance with the rules of his religion may attach to the application a photograph showing him wearing headgear, as long as the facial image is fully visible. In this case, the application shall be accompanied by a statement of the foreigner's religious affiliation. 2. documents confirming: - the purpose of the stay and the need to extend the Schengen visa or the national visa, - possession of sufficient financial resources to cover the costs of subsistence for the entire period of the planned stay in the territory of the Republic of Poland and for the return journey to the country of origin or residence or for the transit to a third country which will grant the entry permit, or the possibility to obtain such resources in accordance with the law, - the credibility of the declaration of the intention to leave the territory of Poland before the expiry of the visa, - possession of health insurance within the meaning of the Act of August 27, 2004. on health care services financed from public funds or travel medical insurance with a minimum insurance amount of 30,000 euros, valid for the period of the foreigner's planned stay in the territory of the Republic of Poland, covering all expenses that may arise during the stay in this territory due to the need to return for medical reasons, the need for urgent medical assistance, emergency hospital treatment or death, in which the insurer undertakes to cover the costs of medical services provided to the insured directly to the entity providing such services, on the basis of a bill issued by this entity - other circumstances stated in the application, - performance of the registration obligation. A foreigner applying for the extension of a Schengen or national visa shall present for inspection a travel document that meets the criteria: 1) its validity will expire no earlier than 3 months after the expiration of the period of validity of the visa applied for ; 2) it contains at least two blank pages; 3) it was issued within the last 10 years. Attachment 1 - Application form for Schengen visa extensionAppendix 2 - Application form for national visa extensionAppendix 3 - RODO Information clauseAppendix 4 - RODO Information clause of the Head of the Office for Foreigners.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://centrumverte.pl/blog/rozliczenie-cudzoziemca-w-polsce-pit-11-czy-ift-1r/</t>
+          <t>https://www.gov.pl/web/uw-pomorski/przedluzenie-wizy-pobytowej</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>We value user privacy
-We use cookies to improve your browsing experience, display ads or customized content, and analyze site traffic. Clicking the "Accept All" button indicates your consent to our use of cookies.
-We use cookies to help users navigate and perform certain functions efficiently. For details on all cookies corresponding to each consent category, see below.
-Cookies classified as "essential" are stored in the user's browser because they are necessary to enable basic site functions.... Show more
-Necessary cookies are essential for the basic functions of the site and the site will not function as intended without them.These cookies do not store any personally identifiable information.</t>
+          <t>The information contained in this charter is not a source of law. They are only of a general and instructional nature. An application for extension of a national visa must be submitted no later than the last day of the visa's validity. A national visa may be extended once, but the period of stay under an extended national visa may not exceed the period of stay prescribed for a national visa, i.e. 1 year. Legal basis: chapter 2 of section IV of the Law of December 12, 2013 on foreigners and Article 33 of Regulation No. 810/2009 of the European Parliament and of the Council of July 13, 2009 establishing a Community Code on Visas.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>How can I report an employer who does not pay my salary in Lower Silesia?</t>
+          <t>How can I register the birth of my child in Polish?</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.sdworx.pl/pl-pl/blog/place/nieterminowa-wyplata-wynagrodzenia</t>
+          <t>https://www.gov.pl/web/gov/zglos-urodzenie-dziecka</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Home&gt;
-Blog&gt;
-Payroll&gt;
-What if the employer is late with payment? The consequences of not paying wages on time
-Pay is a priority for 55% of employees worldwide. Unfortunately, nearly 30% of middle and senior managers admit that they are often - or always! - are underpaid, according to ADP Research Institute's "People at Work 2024: A Global Workforce View" report. Payroll errors are among the many problems workers face. The PIP (State Labor Inspectorate) received about 16,000 complaints related to the payment of wages and other benefits in 2023. What action can an employee take when an employer is late with payment? Check the consequences of late payment of wages on legal grounds.</t>
+          <t>If you have a baby, you need to report it to the appropriate registry office . The head of the office will register the birth of the child, give you its PESEL number and register it. Find out how to report the birth of a child - online or in the office. If you want to report the birth of a child online - you need a trusted profile or an e-card. They allow you to confirm your identity. Check out how to set up a trusted profile or how to use an e-proof.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.gazetaprawna.pl/praca/artykuly/9722231,mobbing-w-polsce-najnowsze-dane-pip.html</t>
+          <t>https://www.gov.pl/web/cyfryzacja/rejestracja-narodzin-dziecka-online</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advertising
-The State Labor Inspectorate has summarized key data on bullying. In 2024, 1,367 pieces of legal advice were given in this area, compared to 829 pieces of advice given in 2023. What did employees ask most often?
-As reported, employees' concerns revolved around problems related to collecting evidence of its occurrence in the work environment or internal procedures. Employees also asked about the possibility of obtaining support from inspectors or the issue of pursuing such claims in court.
-The inspectorate, as stated in the communiqué, also supports victims of bullying when they decide to take legal action and want to obtain compensation for the harm they have suffered.
-</t>
+          <t>A trusted profile and a few minutes - that's all it takes to register the birth of a child online. The new service was launched on June 1, 2018. - It is a gift for Children's Day from the Ministry of Digitization. Parents have 21 days to register their child's birth from the day the birth card is issued. Until now, they had only one option - a visit to the office. From now on they will have a choice - to rush to the office or spend this time with their new family member. Simpler, faster and more convenient - this is the shortest description of the service being launched. How to use it? The whole process is 5 simple steps.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://poradnikpracownika.pl/-niewyplacone-wynagrodzenie-za-prace-czyli-jak-odzyskac-nalezna-wyplate</t>
+          <t>https://www.gov.pl/web/cyfryzacja/co-jest-potrzebne-by-zglosic-narodziny-dziecka-imie-i-internet</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Employee Handbook
-EARNINGS
-Salaries
-Unpaid salary for work, or how to recover the payment due</t>
+          <t>What is needed to report the birth of a child? A name and... the Internet! Johnny, Bozydar, Grześ, Kociemir - choosing a name for a child is not always easy. It is very simple, instead, to report the birth of a new family member. The easiest and fastest way to do this is via the Internet - on GOV.pl. Starting today on TV and the Internet, you can watch our latest spot, in which we encourage you to take advantage of this opportunity. This is another installment of our "e-Poland can!" campaign.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>What should be included in my employment contract in Lower Silesia?</t>
+          <t>How to nostrify a diploma in Poland?</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.bankier.pl/wiadomosc/Umowa-o-prace-wszystko-co-powinienes-o-niej-wiedziec-700002.html</t>
+          <t>https://nawa.gov.pl/uznawalnosc/informacje-dla-uczelni/nostryfikacja-dyplomow</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>An employment contract obliges both parties, i.e. the employee and the employer, to fulfill certain obligations to each other. Each party to the contract
-is also entitled to certain privileges. In turn, the types of employment contracts are different. Employee
-should become well acquainted with the regulations governing the conclusion of labor relations
-labor relations to avoid mistakes and misunderstandings.
-When signing an employment contract,
-we undertake to perform a certain type of work for the employer
-and under his direction. The other party to the contract, the employer, undertakes to
-provide the employee with remuneration for the work. However, one cannot speak of an employment relationship
-employment if certain prerequisites have not been met, such as subordination of the
-of the employee to the employer's instructions, provision of work in person, performance of work
-work for remuneration, at the place and time designated by the employer.
-An important factor is also the repetitive nature of the performance of work and the burden on the
-employer of the risk of conducting business and employing people.
-As of 2016, the Labor Code distinguishes three types of employment contracts: probationary, fixed-term and permanent.
-The Labor Code also distinguishes several
-types of employment contracts. The first of these is a contract
-for a trial period, which is intended to test the employee's qualifications in practice
-practice. It allows the employee to familiarize himself with the conditions and organization of work
-work in a given company. However, it should be remembered that employment on its basis
-cannot last longer than 3 months. The second type of employment contract, is a fixed-term contract. Changes to the undertaking of this type of contract were introduced in 2016. As a result of the changes, it is not possible to enter into a fixed-term contract of any length. Currently, such a contract cannot be entered into for more than 33 months between the same employer and employee. Another change is the limit of fixed-term contracts - after 2016, a maximum of 3 such contracts can be concluded, if exceeded, the employee is considered to be employed for an indefinite period. The said limit does not apply to fixed-term contracts, as mentioned below.
-Z
-From the employee's point of view, however, the most favorable contract is an indefinite term contract, which provides the greatest protection against dismissal
-dismissal. It can be terminated without notice only for legitimate reasons</t>
+          <t>1 What is nostrification Нострифікація дипломів про вищу освіту Nostrification is a procedure leading to the determination of the Polish equivalent of a foreign diploma. Nostrification is subject to a diploma of study abroad, which cannot be recognized as equivalent to the corresponding Polish diploma and professional title on the basis of an international agreement determining equivalence . The nostrification procedure is carried out on the basis of the Regulation of the Minister of Science and Higher Education of September 28, 2018 on the nostrification of diplomas of completion of studies abroad and on the confirmation of completion of studies at a specific level</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://poradnikprzedsiebiorcy.pl/-umowa-o-prace</t>
+          <t>https://www.gov.pl/web/zdrowie/uzyskaj-nostryfikacje-dyplomu-szkoly-wyzszej1</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Human Resources Service
-Labor Law
-Employment contract - learn the basic information
-employment contract</t>
+          <t>If you have a university diploma obtained in a country outside the European Union, you can recognize it as equivalent to its Polish equivalent. Nostrification of diplomas that confirm qualifications to practice medical professions is handled by medical universities - authorized to award the degree of Doctor of Medical Sciences. Note: If you have obtained a diploma abroad confirming the completion of higher education, to which you were referred in accordance with the regulations in force in this regard, the diploma will be recognized without nostrification proceedings.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://hrappka.pl/blog/umowa-o-prace-wzor</t>
+          <t>https://nawa.gov.pl/uznawalnosc/podjecie-pracy-w-polsce/dyplom-z-innego-kraju</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>An employer who intends to hire an employee on the basis of an employment relationship is obliged to sign an employment contract with him. It should contain information about both the employer (company name, TIN, address, representative person) and the employee (name, surname, place of residence). The employment contract is concluded for a probationary, fixed or indefinite period.
-Data for the contract is usually collected using a personal questionnaire. The fastest way is to send a questionnaire for employment using a personnel and payroll system. With this, the prospective employee himself will complete his data for the contract. A profile of the employee will be created, into which data from the questionnaire will be automatically downloaded. Similarly with the contract - there is no need to manually rewrite the data.
-An additional advantage of concluding an employment contract with the help of a suitable system is that it saves time when submitting the document for signature. Using an electronic signature, for example, we can quickly establish an employment relationship, thereby speeding up the start date.
-&gt;&gt; Test the HR and payroll system free of charge.
-Topics covered in the article:</t>
+          <t>A higher education diploma or professional title obtained abroad may be recognized as equivalent to a Polish equivalent on the basis of an international agreement, and in the absence of such an agreement - by nostrification. Diplomas obtained abroad cannot be recognized in Poland if: the institutions that issued them or the institutions in which the education was provided: were not accredited universities on the date of issuance of the diploma or provided a study program that was not accredited on the date of issuance of the diploma; do not operate in the higher education system of any country;</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Can a foreigner open a company in Lower Silesia?</t>
+          <t>How can I get a PESEL for tax purposes in Polish?</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://przybysz.duw.pl/cudzoziemcy-pobyt/zezwolenia-na-pobyt-czasowy/dzialalnosc-gospodarcza/</t>
+          <t>https://www.gov.pl/web/gov/uzyskaj-numer-pesel-dla-cudzoziemcow</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Who makes the request?
-When should I/we submit the application?
-How do I submit an application?
-What documents do I need to submit?
-What are the fees?</t>
+          <t>If you are a foreigner who lives in Poland, you can register - then you will automatically get a PESEL number. If you can't register and some office requires you to get a PESEL number - apply. Check out how to do it. Expand the text Who can get You will get a PESEL number from the office - if you register in Poland for a stay of more than 30 days. Submit an application to any municipality office - if you can't register and need a PESEL number. You will get a PESEL number from the office - if you register in Poland for a stay of more than 30 days.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.migrant.info.pl/pl/strona-glowna-2/dzialalnosc-gospodarcza/mozliwosc-prowadzenia-dzialalnosci-gospodarczej-przez-cudzoziemcow</t>
+          <t>https://www.podatki.gov.pl/abc-podatkow/wyjasnienia/od-1-maja-cudzoziemcy-moga-wystapic-o-nadanie-pesel-do-celow-podatkowych/</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-We would like to draw your attention to the fact that the information provided on this website is not a source of law. We assure you that we have made every effort to comply with the applicable regulations. However, please note that this site is for informational purposes only, and the information on this site cannot be used as a basis in disputes with government authorities. If in doubt, we recommend that you contact the body conducting the administrative proceedings in a given case and familiarize yourself with the provisions of the law that may have a decisive impact on its resolution. We also invite you to contact the migrant.info hotline we run - +48 22 490 20 44
-We would like to draw your attention to the fact that the information provided on this website is not a source of law. We assure you that we have made every effort to comply with applicable regulations. However, please note that this site is for informational purposes only, and the information on this site cannot be used as a basis in disputes with government authorities. If in doubt, we recommend that you contact the body conducting the administrative proceedings in a given case and familiarize yourself with the provisions of the law that may have a decisive impact on its resolution. We also invite you to contact the migrant.info hotline we run - +48 22 490 20 44</t>
+          <t>As of June 1, foreigners can apply for a PESEL for tax purposes On June 1, 2021, an amendment to the Law on the Principles of Registration and Identification of Taxpayers and Payers comes into force regarding the definition of taxpayers whose tax identifier is a PESEL. Thanks to the new regulations, municipal offices will be able to assign a PESEL number to foreigners upon their request.</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://symfonia.pl/blog/rozwoj-firmy/jdg/zakladanie-jednoosobowej-dzialalnosci-w-polsce/</t>
+          <t>https://www.gov.pl/web/uw-warminsko-mazurski/jestes-cudzoziemcem-potrzebujesz-pesel-lub-nip-do-zalatwienia-spraw-podatkowych</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Consent
-Details
-[#IABV2SETTINGS#]
-About cookies
-We use cookies to personalize content and advertising, to offer social features and to analyze traffic on our site. We share information about how you use our site with social, advertising and analytics partners. Partners may combine this information with other data they receive from you or obtain when you use their services.</t>
+          <t>Are you a foreigner? You need a PESEL or NIP to handle tax matters The Head of the Olsztyn Tax Office reminds foreigners of the obligation to have a tax identifier, i.e. a PESEL or NIP number. How to obtain such documents? About it in the following part of the article. If you are a foreigner who lives in Poland, you can register - then you will automatically get a PESEL number. If you can't register, and some office requires you to get a PESEL number - apply. Check how to do it.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>What are the tax requirements for self-employed foreigners in Lower Silesia?</t>
+          <t>How to open a bank account in Poland?</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.ksiega-podatkowa.pl/akademia-skp/rozliczenie-wynagrodzenia-cudzoziemcow</t>
+          <t>https://sip.lex.pl/akty-prawne/mp-monitor-polski/ogolne-zasady-otwierania-i-prowadzenia-rachunkow-bankowych-16820548</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Recently, more and more citizens of other countries have been coming to our country for work purposes. Employing them can be beneficial for Polish entrepreneurs, given the recent difficulties in finding workers among our country's citizens, who themselves also emigrate to the territories of other countries. So if you employ or intend to employ foreigners and want to properly account for their wages and prepare the necessary documentation, be sure to read the following article.
-Before you start recording the wages of foreigners, follow the steps below:
-1. check the residency status of the employed foreigner
-2. ask him/her if he/she has a certificate of residence of a country other than Poland
-3. verify the existence of a double taxation treaty with the country whose residence certificate
-is held by the person in question
-4. select the appropriate type of agreement, calculate the relevant wages and prepare the necessary documentation
-So, one by one...
-Who should be considered a resident?
-A resident is a person who stays in Poland in a given tax year for more than 183 days or who has a center of life interests in our country, e.g. lives here with his family, children go to school here or runs a business. It is sufficient that one of these conditions is met for a foreigner to be considered a resident. Thus, if a foreigner employed by us stays in Poland for a short period of time or has a resident certificate from another country, he cannot be considered a resident.
-Possession of a certificate of residence
-A certificate of residency is basically a confirmation of the fact that the taxpayer is a resident. It is in which country he obtains the certificate that he settles his income. This is because he himself decides where he wants to live and where to pay taxes. A foreigner can also obtain a Polish certificate of residence. To do so, he must apply to the Polish office for its issuance, and the office decides whether to recognize the taxpayer in question as a resident of our country or not. Thus, if our potential employee presents such a certificate, it will entail certain consequences in the calculation of income tax.</t>
+          <t>General rules for opening and maintaining bank accounts. ORDINANCE OF THE PRESIDENT OF THE NATIONAL POLISH BANK dated December 10, 1982 on general rules for opening and maintaining bank accounts. If you want to have access to all related documents, log in to LEX Not yet using LEX programs? Order test access "</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://hrappka.pl/blog/cudzoziemcy/pit-11-czy-ift-1r-jak-rozliczyc-cudzoziemca</t>
+          <t>https://www.knf.gov.pl/dla_rynku/procesy_licencyjne/bankowy/banki/wstep</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>January is an important month for employers. They are obliged to provide the Tax Office with the relevant tax returns. When employing people from Poland, the matter is obvious - the employer issues a PIT-11. However, doubts arise when employing foreigners. How to account for individuals who do not reside in Poland? What annual declaration should be issued to a foreigner employed on the basis of a statement of entrustment of work to a foreigner or on the basis of a work permit? We answer in the article.
-&gt;&gt; Test your HR and payroll system for free
-Issues raised in the article:
-The first and most important step is to determine the tax residency of a foreigner. It determines which country should be the first to pay tax on income.
-For tax purposes, a Polish tax resident is a person who lives in Poland for more than 183 days a year, or a person who resides here for a shorter period, but has a center of personal, life and economic interests in Poland. Such a person is subject to so-called unlimited tax liability.</t>
+          <t>Banking activities and other activities permitted for banks Forms of activity State-owned bank Bank in the form of a joint-stock company Cooperative bank Mortgage bank Requirements applicable to the formation of a bank Introduction Founders Initial capital Bank's own funds Persons scheduled to take up positions Plan of operations of the bank Premises provided for the conduct of the business</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://hrappka.pl/blog/pit-11-dla-cudzoziemca-jaki-urzad-skarbowy</t>
+          <t>https://www.knf.gov.pl/dla_rynku/procesy_licencyjne/bankowy/banki/wymagania_obowiazujace_przy_tworzeniu_banku</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Issues addressed in the article:
-There are two solutions related to accounting for a foreigner in Poland. They depend on whether the foreigner employed in Poland has resident or non-resident status.
-In this case, the declaration should be sent to the tax office for foreigners, and the foreigner's foreign address should be entered.
-The declaration of a resident foreigner should be sent to the tax office in accordance with his place of residence. (The foreigner's foreign address should be entered in the foreigner's address. If the foreigner no longer lives in Poland then the declaration should be sent to his current foreign address. Tax offices remain the same.)
-See our article for more on which tax return to issue to foreigners.</t>
+          <t>Requirements applicable to the establishment of a bank - Financial Supervisory Commission Premises provided for business To facilitate the use of the service, the mechanism that manages it uses cookie technology - information is recorded by the Office's server on the user's computer. It is not used to obtain any data about visitors to the site. The user can disable the option to accept cookies in their web browser at any time. This may cause some difficulties in using the site. For more information, see the Privacy Policy tab. Privacy Policy</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>How can I register a company in Lower Silesia?</t>
+          <t>What are the tax requirements for self-employed foreigners in Poland?</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://dc.biz.pl/wirtualne-biuro-wroclaw-gajowice-2/</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00806</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Consent
-Details
-[#IABV2SETTINGS#]
-About cookies
-Essential 2 Essential cookies contribute to the usability of the website by enabling basic functions such as site navigation and access to secure areas of the website. A website cannot function properly without these cookies.Cookiebot1Learn more about this providerCookieConsentStores the user's cookie consent state for the current domainMaximum retention period: 1 yearName: HTT cookiePGoogle1Learn more about this providerSome of the data collected by this provider is used to personalize and measure the effectiveness of advertising.test_cookieUsed to check if the user's browser supports cookies.Maximum retention period: 1 dayName: HTTP cookie</t>
+          <t>Who can do business in Poland Citizens of the European Union member states and the European Economic Area who want to do business in Poland can: set up their own sole proprietorship or any commercial company</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/watch?v=9EnRI4hflKM</t>
+          <t>https://www.biznes.gov.pl/pl/portal/0613</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-New
-New
-</t>
+          <t>Who can do business in Poland Polish regulations provide for a great deal of freedom in business, which means that in most cases you can set up a company and run it in the form you choose. Read when you need to meet additional conditions. Find out if a company can be opened by a foreigner, a minor or a pensioner. Foreigner's company Setting up a sole proprietorship Polish legislation provides for a great deal of freedom in business, which means that in most cases you can set up a company and run it in the form of your choice. Read when you need to meet additional conditions. Find out if a foreigner, a minor or a pensioner can open a company. How to delegate employees to Poland in the framework of the provision of services Find out what delegation in the framework of the provision of services consists of, what are the rules and obligations of delegating employers, when an employee is a delegated employee. Foreigner's company Delegation Obligations of the employer Employment of an employee</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://www.nieruchomosci-online.pl/porady/dzialalnosc-gospodarcza-w-mieszkaniu-lub-domu-30970.html</t>
+          <t>https://www.biznes.gov.pl/pl/portal/001466</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Sign in
-Buying
-Sale
-Renting</t>
+          <t>A citizen of Ukraine who resides in Poland legally and has a PESEL number may establish a business on the same terms as a Polish citizen in any form. a sole proprietorship - i.e., a business activity of a natural person - and register it with the CEIDG a partnership or a corporation - including a general partnership and a partnership - and register it with the National Court Register.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Do I have to pay taxes in Lower Silesia if I work remotely for a foreign company?</t>
+          <t>Do I have to pay taxes in Polish if I work remotely for a foreign company?</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://www.podatnik.info/publikacje/podatek-za-prace-za-granica-kiedy-nie-trzeba-wykazywac-dochodow-z-zagranicy,6164b0</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00399</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>We and our vendors (2) use cookies and similar technologies to read, store, and write information on your device. Essential cookies are necessary for our site to work properly. With your consent, we and our vendors may also use non-essential cookies to improve user experience, personalize advertisements, and analyze website traffic. For these reasons, we may process your personal data (such as IP address or browsing and interaction data).
-By clicking "Accept," you agree to our website's data use as described in our "Cookie Policy." You may change or withdraw your consent at any time by clicking the "Consent Preferences" link in the footer and accessing the categories, purposes, and vendors tabs.
-We process data for the following purposes and special features: Actively scan device characteristics for identification, Create profiles for personalised advertising, Create profiles to personalise content, Develop and improve services, Measure advertising performance, Measure content performance, Store and/or access information on a device, Understand audiences through statistics or combinations of data from different sources, Use limited data to select advertising, Use limited data to select content, Use profiles to select personalised advertising, Use profiles to select personalised content.
-FREE PROGRAM FOR PIT 2024/2025
-Working abroad often involves earning a higher income than in Poland, which makes it an attractive option for many people. However, it is worth remembering that earnings earned outside Poland may give rise to tax obligations in the country, including the need to settle accounts with the tax authorities in accordance with Polish regulations. In this article, we address the frequently encountered issue of working abroad vs. tax in Poland. We invite you to read on.</t>
+          <t>Cross-border services are services provided to customers from other EU countries. You provide cross-border services when: you move to another country to perform a service, for example, you renovate a building in France you move to Member State A to perform a service for an entity in Member State B, for example, you advise a German entrepreneur on a transaction in the Czech Republic</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://poradnikprzedsiebiorcy.pl/-skladanie-zeznan-podatkowych-przez-nierezydentow</t>
+          <t>https://biznes.gov.pl/pl/portal/00586</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Accounting Service
-Reporting
-Filing of tax returns by non-residents
-Filing of tax returns by n...</t>
+          <t>Poles, as part of the European Union's single internal market, enjoy free movement of goods, services, capital and people - they can trade and do business in all member states of the European Union and the European Economic Area. European Union member states are: Austria, Belgium, Bulgaria, Croatia, Cyprus, Czech Republic, Denmark, Estonia, Finland, France, Germany, Greece, Hungary, Ireland, Italy, Latvia, Lithuania, Luxembourg, Malta, Netherlands, Poland, Portugal, Romania, Slovenia, Slovakia, Spain, Sweden. Member countries of the European Economic Area, in addition to those of the European Union, are: Norway, Iceland, Liechtenstein.</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://www.podatki.biz/i91099/podatek-dochodowy-osob/podatek-dochodowy-osob.htm</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00229</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>mypodatki.biz
-REGISTRATION
-MENU
-Thematic sections
-News - taxes, accounting, Social Security, economyABC - law and taxes for beginnersAmortization - fixed assets and intangible assetsFor tax readers.bizBusiness activityVAT invoicingTax forms and document templatesFiscal cash registersDeductible costsLimits, parameters, indicatorsPC tax, real estate tax, other taxes and feesVAT and excise taxes - general issuesPIT and CIT income taxes - general issuesEmployees: hiring, vacations, benefits, allowances, equivalentsAccounting: PKPiR | Full accounting | Tax and accounting recordsAnnual settlement of PITRata from registered income and tax cardCar in the companyEveryday issues: inheritances and donations, private lease, real estate, buying and sellingTraining starting in the coming daysSocial security contributions: social insurance, health insurance, FP, FGŚPTax obligations, that is, how to pay taxes
-News - taxes, accounting, Social Security, economy</t>
+          <t>Where to pay taxes is determined by the principle of residency, or tax residence. Individuals who are resident for tax purposes in Poland , have unlimited tax liability. That is, they settle all income here, both earned in Poland and abroad. An individual who meets at least one of the two conditions has domicile in Poland:</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>How can I get a PESEL for tax purposes in Lower Silesia?</t>
+          <t>How to use the public health service in Poland?</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://poradnikprzedsiebiorcy.pl/-pit-11-za-cudzoziemca-wylacznie-z-numerem-pesel</t>
+          <t>http://pacjent.gov.pl/zasady-korzystania-z-systemu</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-According to the expert
-PIT-11 for a foreigner vs. tax identifier
-pit-11 for a foreigner
-4.93/5
-(30)</t>
+          <t>When and under what conditions can you benefit from the health care system? Here are the answers</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://hrappka.pl/blog/cudzoziemcy/pit-11-czy-ift-1r-jak-rozliczyc-cudzoziemca</t>
+          <t>http://pacjent.gov.pl/system-opieki-zdrowotnej</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>January is an important month for employers. They are obliged to provide the Tax Office with the relevant tax returns. When employing people from Poland, the matter is obvious - the employer issues a PIT-11. However, doubts arise when employing foreigners. How to account for individuals who do not reside in Poland? What annual declaration should be issued to a foreigner employed on the basis of a statement of entrustment of work to a foreigner or on the basis of a work permit? We answer in the article.
-&gt;&gt; Test your HR and payroll system for free
-Issues raised in the article:
-The first and most important step is to determine the tax residency of a foreigner. It determines which country should be the first to pay tax on income.
-For tax purposes, a Polish tax resident is a person who lives in Poland for more than 183 days a year, or a person who resides here for a shorter period, but has a center of personal, life and economic interests in Poland. Such a person is subject to so-called unlimited tax liability.</t>
+          <t>The most important links in the health care system in Poland are the practices of doctors, nurses and midwives, clinics and hospitals. To some of them we can go without a referral, to others we need such a document Find out how health care is organized in Poland. The first tier, or primary health care</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://poradnikprzedsiebiorcy.pl/-oswiadczenie-cudzoziemca-o-rezydencji-podatkowej-wzor-do-pobrania</t>
+          <t>http://pacjent.gov.pl/aktualnosc/wiesz-jak-dziala-system-ochrony-zdrowia</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Download
-Sample letters
-Statement of foreigner's tax residency - downloadable template
-Foreigner's statement of tax residency...</t>
+          <t>Learn the rules of the health care system in order to take advantage of it People who are compulsorily insured, voluntarily insured or meet other conditions, as stipulated by law, are entitled to systemic care. You can check your insurance status on the Internet Patient Account.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>What are the health care and social insurance premiums for foreigners in Lower Silesia?</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
+          <t>How can I apply for Polish citizenship in Poland?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/mswia/uzyskaj-polskie-obywatelstwo</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Confirmation of possession or loss of Polish citizenship Want to get Polish citizenship? Have you lost your Polish citizenship and want to regain it? Do you need official confirmation that you have Polish citizenship? Here you will find all the information you need. Apply to the President for Polish citizenship</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://poradnikpracownika.pl/-skladki-odprowadzane-od-wynagrodzenia</t>
+          <t>https://powroty.gov.pl/nabycie-obywatelstwa-polskiego-10000</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Employee Handbook
-EMPLOYMENT
-Insurance
-Contributions paid by employer and employee on wages in 2025.</t>
+          <t>Information according to the legal status as of: 2024-09-11 The issues of acquiring Polish citizenship and losing it are regulated by the Act of April 2, 2009 on Polish citizenship. 1. birth from parents, at least one of whom has Polish citizenship - the rule of blood/Ius Sanguinis</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://tuz.pl/ekspert-radzi/ubezpieczenie-zdrowotne-dla-cudzoziemcow-w-polsce-wszystko-co-musisz-wiedziec-na-ten-temat/</t>
+          <t>https://archiwum.mswia.gov.pl/pl/bezpieczenstwo/obywatelstwo-i-repatri/cudzoziemcy/10169,SPOSOBY-NABYCIA-OBYWATELSTWA-POLSKIEGO.html</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>As a member of the European Union, Poland offers a wide range of health services to its citizens. However, for foreigners temporarily or permanently residing in Poland, health insurance issues can be a bit more complex. For those arriving in Poland, it is important to understand the rules, types of insurance and procedures related to health care. Below you will find all the relevant information on this subject.
-Medical expenses insurance for foreigners is a voluntary policy that provides financial protection in the event of a sudden illness or accident while in Poland. It is especially important for people who are not covered by public health insurance in Poland, such as citizens of third countries. Coverage for a foreigner's medical expenses may vary depending on the policy chosen, but usually includes:
-outpatient and hospital treatment costs,
-costs of medicines and dressings,
-costs of diagnostic tests and surgical procedures,</t>
+          <t>The issues of acquiring Polish citizenship and losing it are regulated by the Act of April 2, 2009 on Polish citizenship . The Act contains two basic principles concerning Polish citizenship. The principle of continuity of Polish citizenship, expressed in Article 2 of the Act, guarantees the permanence of citizenship in time, starting from the moment of its acquisition, in accordance with the provisions in effect at the time, regardless of changes to the legislation concerning citizenship. This means that persons who acquired Polish citizenship on the basis of old laws, subsequently repealed or amended, if they have not lost their Polish citizenship, retain it in accordance with the laws in effect on the date of acquisition. This principle is at the same time a directive to the competent public administration bodies in proceedings to confirm possession or loss of Polish citizenship. On the other hand, the principle of the exclusivity of Polish citizenship, introduced by the provision of Article 3 of the Law, is closely related to the problem of dual citizenship, as it creates a clear conflict directive in the event of its occurrence and allows for the removal of its adverse effects. The draft law adopts the principle of permissibility of multiple citizenships while maintaining the absolute priority of Polish citizenship. A Polish citizen may simultaneously hold Polish citizenship and citizenship of a foreign state, but even then he or she has the same rights and obligations towards the Republic of Poland as a person holding only Polish citizenship, i.e. he or she cannot invoke with legal effect towards the Polish authorities the foreign citizenship held simultaneously or the rights and obligations arising from it. Birth from parents, at least one of whom has Polish citizenship - Rule of blood/Ius Sanguinis</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>What rights do I have as a tenant in Lower Silesia?</t>
+          <t>What taxes do foreigners have to pay in Poland?</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://gazetawroclawska.pl/stancja-wroclaw-jak-wynajac-mieszkanie-poradnik/ar/c3-969554</t>
+          <t>https://www.gov.pl/web/gruzja/srodki-finansowe-wymagane-od-cudzoziemca-wjezdzajacego-do-polski</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>This website is using a security service to protect itself from online attacks. The action you just performed triggered the security solution. There are several actions that could trigger this block including submitting a certain word or phrase, a SQL command or malformed data.
-You can email the site owner to let them know you were blocked. Please include what you were doing when this page came up and the Cloudflare Ray ID found at the bottom of this page.
-Cloudflare Ray ID: 92f5478f88e1c3fe
--
-      Your IP:
-      Click to reveal
-83.27.101.111
--
-Performance &amp; security by Cloudflare</t>
+          <t>Financial resources required of a foreigner entering Poland According to the Decree of the Minister of Internal Affairs of February 23, 2015 on the financial resources required of a foreigner entering the territory of the Republic of Poland and documents that can confirm the possibility of obtaining such resources, as well as the purpose and duration of the planned stay under Article 26 (1) of the Law on Foreigners of December 12, 2013 , a foreigner should have the financial resources to cover the costs of: - subsistence during his/her stay in this territory,</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.flatte.app/blog/obowiazki-wynajmujacego-mieszkanie</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00806</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Obligations of the landlord of an apartment can arise both from the law and from the provisions of the contract. At the same time, the content of the lease agreement must not violate the provisions of the law, nor oppose the nature of the legal relationship or the principles of social intercourse. What if the obligations of the property owner to the tenant detailed in the concluded lease agreement are contrary to the content of the law? As a rule, the principle of freedom of contract applies, but in the case of contradiction of provisions with the content of the applicable law, including, in particular, the Law on the Rights of Tenants, such provisions contained in the contract are invalid, that is, they have no legal effect.
-The law of renting an apartment in Poland, including the obligations of the landlord under the law, are listed primarily in two pieces of legislation. The first is the Law of June 21, 2021 on the protection of tenants' rights, the housing stock of the municipality and amendments to the Civil Code. The second is the Civil Code, and more specifically the provisions in Section I. Knowledge of the aforementioned pieces of legislation is essential when creating a lawful lease agreement.
-Undeniably, the primary obligation of the landlord of an apartment is to deliver the premises to the tenant. The apartment must be in a condition as agreed and ready for use. The landlord is also obliged to allow the tenant to use the premises. In practice, this means the obligation to issue the keys to the premises on the agreed date. Another obligation of the landlord is to determine the amount of rent and additional fees. It is worth remembering that it is also the investor's duty to write down the status of the meters and the handover protocol. Another obligation of the landlord, which landlords often forget, is to show the tenant the energy performance certificate for the premises.
-These are not the only obligations of the property owner to the tenant. According to the law, the obligations of a residential landlord also include ensuring the proper operation of existing equipment and installations. In particular, those related to the real estate, which enable the tenant to use water, electricity and gaseous and liquid fuels, heat, passenger lifts and other installations and equipment of the premises and building specified by separate regulations.
-It is obvious that both equipment and appliances are subject to breakdown and wear and tear. This necessitates their repair or replacement. As long as the owner of the apartment is also its tenant, there is no problem in determining who is responsible for such maintenance and repairs. The problem arises in the case of rented apartments. There, on the one hand, there is the owner of the apartment, and on the other - the tenant who resides in that apartment. Who, then, is responsible for repairs and renovations in a rented apartment? According to the law, the obligation of the landlord to ensure the smooth operation of the equipment and installations related to the apartment does not mean that he is responsible for all repairs. The developer is responsible for some of the repairs, and the tenant is responsible for the rest. So what repairs is the landlord responsible for, and what repairs is the tenant responsible for?</t>
+          <t>Who can do business in Poland Citizens of the European Union member states and the European Economic Area who want to do business in Poland can: set up their own sole proprietorship or any commercial company</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://skup.io/czy-lokator-moze-nie-wpuscic-wlasciciela/</t>
+          <t>https://www.gov.pl/web/armenia/srodki-finansowe-wymagane-od-cudzoziemcow-wjezdzajacych-do-polski</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>We value user privacy
-We use cookies to improve your browsing experience, display ads or customized content, and analyze site traffic. Clicking the "Accept All" button indicates your consent to our use of cookies.
-We use cookies to help users navigate and perform certain functions efficiently. For details on all cookies corresponding to each consent category, see below.
-Cookies classified as "essential" are stored in the user's browser because they are necessary to enable basic site functions.... Show more
-More information on how cookies from third parties work and how we handle your data is provided in:  Google's privacy policy</t>
+          <t>Financial resources required of foreigners entering Poland According to the Decree of the Minister of Internal Affairs of February 23, 2015 on the financial resources required of a foreigner entering the territory of the Republic of Poland and the documents that can confirm the possibility of obtaining such resources, as well as the purpose and duration of the planned stay under Article 26 (1) of the Law on Foreigners of December 12, 2013 , each foreigner should have the financial resources to cover the costs of: subsistence during his stay in this territory;</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Can a landlord evict me without notice in Lower Silesia?</t>
+          <t>How to register in Poland?</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://gazetawroclawska.pl/najem-mieszkania-o-czym-nalezy-pamietac/ar/11984540</t>
+          <t>https://www.gov.pl/web/gov/zamelduj-sie-na-pobyt-staly-lub-czasowy-dluzszy-niz-3-miesiace</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>This website is using a security service to protect itself from online attacks. The action you just performed triggered the security solution. There are several actions that could trigger this block including submitting a certain word or phrase, a SQL command or malformed data.
-You can email the site owner to let them know you were blocked. Please include what you were doing when this page came up and the Cloudflare Ray ID found at the bottom of this page.
-Cloudflare Ray ID: 92f54809bf17c3fe
--
-      Your IP:
-      Click to reveal
-83.27.101.111
--
-Performance &amp; security by Cloudflare</t>
+          <t>Register for permanent or temporary residence longer than 3 months Are you changing your place of residence? Or are you returning from abroad and don't have a registration in Poland? Remember to register. You can do it online or at the municipality office. If you are a Polish citizen and your child was born in Poland - the head of the civil registry office that prepared the birth certificate will register your child ex officio.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://skup.io/kiedy-nie-mozna-wyrzucic-lokatora-z-mieszkania/</t>
+          <t>https://www.gov.pl/web/cyfryzacja/zamelduj-sie-wygodnie--przez-internet</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>We value user privacy
-We use cookies to improve your browsing experience, display ads or customized content, and analyze site traffic. Clicking the "Accept All" button indicates your consent to our use of cookies.
-We use cookies to help users navigate and perform certain functions efficiently. For details on all cookies corresponding to each consent category, see below.
-Cookies classified as "essential" are stored in the user's browser because they are necessary to enable basic site functions.... Show more
-More information on how cookies from third parties work and how we handle your data is provided in:  Google's privacy policy</t>
+          <t>Are you changing your place of residence? If so, you certainly have a lot on your mind, and a visit to the office is the last thing on your mind right now. We have good news - thanks to our e-services, you'll be able to handle registration matters from your armchair, or even a hammock. This is not only convenient, but also a popular solution. In May alone, Poles used e-registration services 20,815 times. In turn, throughout last year - more than 180,000 times. It's already easy to register online. Soon it will be even easier! And how to use e-registration services? Let's start with what you will need.</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://pogorzelski.pl/eksmisja-z-mieszkania-czy-mozna-wyrzucic-lokatora-z-mieszkania/</t>
+          <t>https://www.gov.pl/web/gov/zamelduj-sie-na-pobyt-staly-dla-cudzoziemcow</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>We value user privacy
-We use cookies to improve your browsing experience, display ads or customized content, and analyze site traffic. Clicking the "Accept All" button indicates your consent to our use of cookies.
-We use cookies to help users navigate and perform certain functions efficiently. For details on all cookies corresponding to each consent category, see below.
-Cookies classified as "essential" are stored in the user's browser because they are necessary to enable basic site functions.... Show more
-Essential cookies are critical to the basic functions of the site and the site will not function as intended without them. These cookies do not store any personally identifiable information.</t>
+          <t>Register for permanent or temporary residence To find out how to register for permanent or temporary residence, answer the questions below. If you live in Poland - register for permanent or temporary residence .</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>How do I get my rental deposit back in Lower Silesia?</t>
+          <t>Can I open a bank account in Polski as a foreigner?</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://ladek.pl/ogloszenie-o-ii-naborze-na-najem-w-ramach-sim-sudety-2-nabor/</t>
+          <t>http://bip.brpo.gov.pl/pl/content/k%C5%82opoty-cudzoziemca-z-kontem-w-polskim-banku</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Home
-NEWS
-INFORMATION
-...
-Announcement of the 2nd call for rent under SIM SUDETY</t>
+          <t>An Iranian citizen cannot open a bank account in Poland, even though he has a temporary residence card in Poland, has been studying and working here for several years, and his wife is Polish. He presented his problem to the RPO's Field Office in Wroclaw. The Ombudsman's attorney sent a letter on his case to the Polish Bank Association and the Office of Competition and Consumer Protection, indicating, among other things, that discrimination may have occurred. The problem was also presented to: the Financial Supervision Commission and the Financial Ombudsman. The case was also handled by the National Bank of Poland, the Financial Supervision Commission and the General Inspector of Financial Information. The Polish Bank Association reasoned: the refusal to open a bank account is due to the need to respect specific restrictive measures and the provisions of the Law of November 16, 2000 on money laundering and terrorist financing. However, the opinion of the National Bank of Poland or the General Inspector of IF shows that there is no basis in the law for refusing to open an account for Iranian citizens. Even taking into account the guidelines and recommendations recognizing the Islamic Republic of Iran as a high-risk country.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://bingowynajem.pl/kaucja-w-umowie-najmu-co-wynajmujacy-moze-potracic-z-kaucji/</t>
+          <t>https://www.prawo.pl/biznes/czy-polacy-moga-zakladac-konta-w-zagranicznych-bankach,514996.html</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>A security deposit in an apartment lease is a safeguard for the landlord of a rental property in the event that the tenant defaults on rent payments or causes damage to equipment or even the property itself. When does the landlord have the right not to return the security deposit? What to do when a landlord refuses to return a security deposit for an apartment without justification? These and other questions are answered in our article today.
-Table of contents
-According to the Law of June 21, 2001 on the protection of tenants' rights, the housing stock of the municipality and the amendment of the Civil Code, the deposit is refundable within one month from the date of vacating the premises or acquiring its ownership by the tenant.
-Although by definition the deposit is refundable, there are several situations in which the landlord has the right to keep it. If the tenant is in arrears on rent or utility bills that exceed the value of the security deposit, it will certainly not be returned. Situations in which the landlord can keep the deposit should be included in the contract. Another reason for not returning the money may be damage to the property and equipment. The condition of the apartment and items at the time of handing over the property should coincide with the condition from the handover protocol. In case of damage, the deposit will be deducted.
-Above we wrote about situations when the landlord has the right not to return the deposit to the tenant. Sometimes a refund is possible if rent arrears or repairs do not exceed the value of the deposit, or if part of the damage has already been covered at the expense of the tenant and this has been documented.</t>
+          <t>You can keep money in an account abroad, but it's not easy everywhere You can keep money in an account abroad, but it's not easy everywhere The war across the eastern border and the weak zloty have prompted people to look around for accounts in foreign banks. And while we don't have to worry about money in our banks these days, accounts abroad have become more tempting.</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://rankomat.pl/nieruchomosci/kaucja-w-umowie-najmu-mieszkania</t>
+          <t>https://www.gov.pl/web/gruzja/srodki-finansowe-wymagane-od-cudzoziemca-wjezdzajacego-do-polski</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Consent
-Details
-[#IABV2SETTINGS#]
-About cookies
-We use cookies and other tracking tools (e.g. Pixel or API) to measure performance, customize our marketing, and provide a better experience on our site.</t>
+          <t>Financial resources required of a foreigner entering Poland According to the Decree of the Minister of Internal Affairs of February 23, 2015 on the financial resources required of a foreigner entering the territory of the Republic of Poland and documents that can confirm the possibility of obtaining such resources, as well as the purpose and duration of the planned stay under Article 26 (1) of the Law on Foreigners of December 12, 2013 , a foreigner should have the financial resources to cover the costs of: - subsistence during his/her stay in this territory,</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Are there any legal restrictions on renting an apartment by a foreigner in Lower Silesia?</t>
+          <t>Can the landlord evict me without notice in Polsky?</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://cudzoziemiec.eu/?q=obrot_cudzoziemcy</t>
+          <t>https://powroty.gov.pl/-/wypowiadanie-umow-najmu-przez-wynajmujacego-wlasciciela-nieruchomosci-wielka-brytania</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Legal residency calculator
-foreigners
-buy
-real estate
-real estate trade</t>
+          <t>It is worth noting that some of the rules regarding the length of notice have changed due to coronavirus . Assured shorthold tenancies - Assured shorthold tenancies A landlord of a rental property may terminate the lease without cause if:</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://sawastian-lipska.pl/blog/czy-cudzoziemiec-moze-kupic-nieruchomosc-w-polsce/</t>
+          <t>https://www.prawo.pl/prawo/kupno-oswiadczenia-o-mozliwosci-zamieszkania-najem-okazjonalny,520257.html</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>660 539 046
-kancelaria@sawastian-lipska.pl
-Return to previous page
-August 4, 2024
-No comments</t>
+          <t>Address "to evict" for 500 zlotys? Occasional lease agreement not so safe Address "to evict" for 500 zł? Occasional lease agreement not so safe The statement needed to conclude the agreement is easy to buy on the Internet - it costs about 400 - 500 zł. This calls into question the whole point of the institution of occasional rental, because in case of a dispute between the parties to the agreement, it can be problematic for both of them.</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://kancelaria-skarbiec.pl/jak-cudzoziemiec-moze-kupic-nieruchomosc-w-polsce-luka-w-ustawie/</t>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/kodeks-cywilny-16785996/ks-3-tyt-17-dz-1</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>We value user privacy
-We use cookies to improve your browsing experience, display ads or customized content, and analyze site traffic. Clicking the "Accept All" button indicates your consent to our use of cookies.
-We use cookies to help users navigate and perform certain functions efficiently. For details on all cookies corresponding to each consent category, see below.
-Cookies classified as "essential" are stored in the user's browser because they are necessary to enable basic site functions.... Show more
-Necessary cookies are essential for the basic functions of the site and the site will not function as intended without them.These cookies do not store any personally identifiable information.</t>
+          <t>A contract for the lease of real estate or premises for a period longer than one year should be concluded in writing. If this form is not observed, the contract shall be deemed to have been concluded for an indefinite period. If during the term of the lease the thing requires repairs, which are borne by the lessor, and without which the thing is not fit for the agreed use, the lessee may set a reasonable time limit for the lessor to perform the repairs. After ineffective expiration of the set time limit, the lessee may make the necessary repairs at the expense of the lessor. If a third party asserts claims against the lessee regarding the leased thing, the lessee shall immediately notify the lessor.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>How can I get married in Lower Silesia as a foreigner?</t>
+          <t>How long can I stay in Poland after my visa expires?</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://tvn24.pl/wroclaw/wroclaw-czekaja-na-legalizacje-w-polsce-rodza-im-sie-dzieci-umieraja-bliscy-st7781158</t>
+          <t>https://migrant.poznan.uw.gov.pl/pl/faq/przedluzenie-wizy</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>TVN24 live
-TVN24 BiS live
-TVN24 in Ukrainian
-TVN24NewsWorldPolandBusinessMeteoPremiumSportsHealthTechnologyCulture and styleInteresting news.
-FactsSee FactsFacts After FactsFacts About the WorldFacts After NoonFacts People.</t>
+          <t>If you plan to stay in Poland after the expiration of your visa for more than 3 months, you should apply for a temporary residence permit. As a rule, you can stay in Poland for tourist purposes on the basis of visa-free movement or a visa. Your total stay on the territory of all Schengen member states without the need for a visa cannot exceed 90 days during any 180-day period. Staying for tourist purposes - extension of visa-free travel</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://www.olsztyn-adwokat.pl/proces-uzyskiwania-zezwolenia-na-staly-pobyt-dla-cudzoziemca-malzonka-obywatela-polski/</t>
+          <t>https://www.gov.pl/attachment/c4067bab-e664-4072-8be5-6c90367ab4e3</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>About the Firm
-Team
-Scope of services ►Family and guardianship casesInheritance and donationsVindication of debtsProtection of debtorsDamages compensation and pensionsProperty lawProtection of property and possessionContractual claims and consumer lawBusiness and commercial lawLabor and social security lawLegal service for entrepreneursCriminal law and misdemeanor lawAdministrative lawAliensMediationServices of uniformed services and Civil Service Corps
-Family and guardianship matters
-Inheritances and donations</t>
+          <t>If you plan to stay in Poland after the expiration of your visa for more than 3 months, you should apply for a temporary residence permit. As a rule, you can stay in Poland for tourist purposes on the basis of visa-free movement or a visa. Your total stay on the territory of all Schengen member states without the need for a visa cannot exceed 90 days during any 180-day period. Staying for tourist purposes - extension of visa-free travel</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://migrant.wsc.mazowieckie.pl/pl/procedury/malzonek-ma-zezwolenie-na-pobyt</t>
+          <t>https://zielonalinia.gov.pl/-/ruch-bezwizowy-ktorych-krajow-dotyczy-</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Go to main menu
-Skip to content
-Availability
-Home page
-Procedures</t>
+          <t>Provisions on visa requirements and visa-free travel when entering any of the member countries should be sought primarily in Regulation 2018/1806 of the European Parliament and of the Council of November 14, 2018, listing third countries whose nationals must have visas when crossing external borders, and those whose nationals are exempt from this requirement. Its Annexes I and II list the countries whose nationals are subject to visa requirements when crossing the external borders of the Member States, and those whose nationals are exempt from the requirement when their total stay does not exceed 90 days during any 180-day period. Annex II of the aforementioned regulation contains a list of third countries whose nationals are exempt from the visa requirement when crossing the external borders of the Member States for a stay of no more than 90 days in any 180-day period. These are: States: Former Yugoslav Republic of Macedonia, Andorra, United Arab Emirates, Antigua and Barbuda, Albania, Argentina, Australia, Bosnia and Herzegovina, Barbados, Brunei, Brazil, Bahamas, Canada, Chile, Colombia, Costa Rica, Dominica, Micronesia, Grenada, Georgia, Guatemala, Honduras, Israel, Japan, Kiribati, Saint Kitts and Nevis, South Korea, Saint Lucia, Monaco, Moldova, Montenegro, Marshall Islands, Mauritius, Mexico, Malaysia, Nicaragua, Nauru, New Zealand, Panama, Peru, Palau, Paraguay, Serbia ), Solomon Islands, Seychelles, Singapore, San Marino, El Salvador, East Timor, Tonga, Trinidad and Tobago, Tuvalu, Ukraine, United Kingdom of Great Britain and Northern Ireland, United States of America, Uruguay, Holy See, Saint Vincent and the Grenadines, Venezuela, Vanuatu, Samoa, Taiwan .</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>What are the requirements for family reunification visas in Lower Silesia?</t>
+          <t>What documents are needed to work in Poland?</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://przybysz.duw.pl/cudzoziemcy-pobyt/zezwolenia-na-pobyt-czasowy/polaczenie-z-rodzina/</t>
+          <t>https://wroclaw.praca.gov.pl/dla-bezrobotnych-i-poszukujacych-pracy/abc-bezrobotnego-i-poszukujacego-pracy/dokumenty-potrzebne-do-rejestracji-osoby-bezrobotnej</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Who makes the request?
-When should I/we submit the application?
-How do I submit an application?
-What documents do I need to submit?
-What are the fees?</t>
+          <t>Identity card or other identity document, such as a passport; a statement regarding the place of registration, whereby if the above statement raises reasonable doubts in the authority, the office may always call for the submission of a registration certificate issued by the registration authority; school graduation certificates, diplomas or other documents confirming qualifications or certificates of completion of training;</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://help.unhcr.org/poland/pl/dostep-do-uslug-dla-uznanych-uchodzcow/laczenie-rodzin/</t>
+          <t>https://www.biznes.gov.pl/pl/portal/ou1611</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>العربية
-English
-Kurdî
-Русский
-Українська</t>
+          <t>Fill out and send an electronic application at praca.gov.pl. You will sign it with a qualified signature or trusted profile. Permit type A or B for work of a foreigner on the territory of Poland Are you an entrepreneur, have a company in Poland and want to hire a foreigner from outside the EU, EEA or Switzerland? You must first obtain a type A or B work permit for him or her. Read how these permits differ and how to obtain them.</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://www.migrant.info.pl/pl/pobyt-w-polsce-czlonkow-rodziny-obywateli-panstw-trzecich</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00210</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-We would like to draw your attention to the fact that the information provided on this website is not a source of law. We assure you that we have made every effort to comply with the applicable regulations. However, please note that this site is for informational purposes only, and the information on this site cannot be used as a basis in disputes with government authorities. If in doubt, we recommend that you contact the body conducting the administrative proceedings in a given case and familiarize yourself with the provisions of the law that may have a decisive impact on its resolution. We also invite you to contact the migrant.info hotline we run - +48 22 490 20 44
-We would like to draw your attention to the fact that the information provided on this website is not a source of law. We assure you that we have made every effort to comply with applicable regulations. However, please note that this site is for informational purposes only, and the information on this site cannot be used as a basis in disputes with government authorities. If in doubt, we recommend that you contact the body conducting the administrative proceedings in a given case and familiarize yourself with the provisions of the law that may have a decisive impact on its resolution. We also invite you to contact the migrant.info hotline we run - +48 22 490 20 44</t>
+          <t>The procedure for obtaining a temporary residence and work permit, i.e. a unified permit, is advantageous because all the formalities legalizing a foreigner's stay and employment take place under a single administrative procedure - the foreigner does not have to apply separately for a residence permit , and the employer - for a work permit. The provincial governor, who has granted a uniform permit for temporary residence and work in the territory of Poland, issues a residence card to the foreigner ex officio. The residence card, during the period in which it is valid, confirms the identity of the foreigner and entitles him, together with a travel document, to repeatedly cross the border without the need to obtain a visa.</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>How can I register the birth of my child in Lower Silesia?</t>
+          <t>How to get a PESEL in Poland?</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://www.mops.wroclaw.pl/10-formy-pomocy?start=27</t>
+          <t>https://www.gov.pl/web/gov/uzyskaj-numer-pesel-dla-cudzoziemcow</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Skip to content Skip to search engine
-Accessibility declaration High contrast A- A+
-Home Page</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>https://narodziny-milosci.pl/niemowle/</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>The child's biological mother is only 15 years old. She is not ready to take care of the baby, nor does she have any support from her immediate family. Mom remains under the care of a doctor, the pregnancy is developing normally.
-A foster family is needed for her baby, who will be born at the end of August (Not adoptive!). The family needs to be aware that until the mother turns 18, the Court will not issue a decision to terminate parental rights and adoption will not be possible until then.
-We are looking for a family that will be prepared for possibly two scenarios. The first is: for the child to be returned to the biological mom when she comes of age, or the second for the child to be adopted if the biological mom is unable to take care of the child.
-We depend on a family that will try to help the mom find her way in her new role, that will show her support (support she cannot count on from her loved ones). Maybe that way she will be able to keep her child in the future.
-People, (especially those who have completed the training on rz and live in Lower Silesia or Greater Poland) and would like to learn more - I invite you to contact us for detailed information: dzieckoadopcyjne@gmail.com - here we always respond the fastest (or on priv on FB).</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>https://mops.wroclaw.pl/10-formy-pomocy?start=30</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Skip to content Skip to search engine
-Accessibility declaration High contrast A- A+
-Home Page</t>
-        </is>
-      </c>
+          <t>If you are a foreigner who lives in Poland, you can register - then you will automatically get a PESEL number. If you can't register and some office requires you to get a PESEL number - apply. Check how to do it.
+Information:
+Expand text
+Who can get
+Get a PESEL number from the office - if you register in Poland for a stay of more than 30 days.
+File an application at any municipality office - if you can't register and need a PESEL number.
+Expand the text
+What you need to prepare
+If you cannot register:
+PESEL number application - open the file in a new window - download and fill it out at home. You can also get it at the municipality office,
+a document that will confirm your identity and other data you enter in the application.
+You can apply in person or an attorney can do it on your behalf. Find out at the office how to handle the matter by proxy.
+Remember! In the application, enter the actual legal basis from which the obligation to have a PESEL number arises. If an office (for example, ZUS or the tax office) requires you to provide your PESEL number - it should also indicate to you the legal basis.
+If there are any deficiencies in the application - you will get a message to fill them in. The office may not process your application - if the application does not meet the official requirements.
+Expand the text
+What you need to do
+Fill out the application and prepare a document that will prove your identity - for more information, see What you need to prepare.
+Submit your application to any municipal office - for more information, see Where you pick up.
+Expand the text
+How much you will pay
+The service is free of charge.
+Expand the text
+How much will you wait
+The official will accept your application right away. If there is a basis for the PESEL number - you will receive a notification of the PESEL number.
+Expand text
+Where will you pick up
+At the municipal office where you apply.
+Expand text
+Legal basis
+Act of September 24, 2010 on population registration (Journal of Laws of 2021, item 510, as amended),
+Regulation of the Minister of Internal Affairs of January 4, 2012 on assigning or changing the PESEL number (Journal of Laws of 2015, item 1984).</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Can I drive in Lower Silesia on a foreign driver's license?</t>
+          <t>What are the rights of an employee in Poland?</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.prawo.pl/ukraina/3,strona.html</t>
+          <t>https://www.gov.pl/attachment/26e5c093-83dd-4b1b-9dd8-a353e0bd18af</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ukraine
-</t>
+          <t>Obligations of the employee and the employer - Labor Code - ZL Sources of labor law - Ministry of Family, Labor and Policy ... Article 100 - Labor Code. - OJ 2025.277 t.j. - OpenLEX</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://www.rynek-kolejowy.pl/wiadomosci/tylko-pesa-chce-sprzedac-dwa-spalinowe-zespoly-trakcyjne-kolejom-dolnoslaskim-97822.html</t>
+          <t>https://www.gov.pl/web/rodzina/podstawowe-informacje-z-zakresu-prawa-pracy</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>PARTNER WEBSITES
-marketinfrastruktury.pl
-transport-publicny.pl
-market-flight.pl
-tor-konferencje.pl
-zdgtor.pl
-Business
-Infrastructure
-Passenger
-Law</t>
+          <t>Remote work The Act of December 1, 2022 on amendments to the Labor Code and certain other laws introduced remote work into the Labor Code, while repealing provisions on telework. The new regulations governing remote work took effect on April 7, 2023. Sobriety control and control for agents acting similarly to alcohol The Act of December 1, 2022 amending the Labor Code and certain other acts introduced into the Labor Code the possibility of sobriety control of employees and control for agents acting similarly to alcohol. The new regulations came into force on February 21, 2023. Working time Working time is one of the most important subjects of labor law regulation. This is because it sets the time limits within which an employer can demand that an employee be ready to provide work.</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://bip.um.wroc.pl/attachments/download/152367</t>
+          <t>https://www.gov.pl/web/rodzina/zrodla-prawa-pracy</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>PARTNER WEBSITES
-marketinfrastruktury.pl
-transport-publicny.pl
-market-flight.pl
-tor-konferencje.pl
-zdgtor.pl
-Business
-Infrastructure
-Passenger
-Law</t>
+          <t>The primary source of labor law is the Act of June 26, 1974. - Labor Code and implementing acts to the Labor Code. Ordinance of the Minister of Family and Social Policy of May 8, 2023 on applications for employees' rights related to parenthood and documents attached to such applications , Ordinance of the Minister of Labor and Social Policy of January 8, 1997 on detailed rules for granting vacation leave, determination and payment of remuneration for the duration of leave and cash equivalent for leave ,</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>How can I exchange my driver's license for a Polish one in Lower Silesia?</t>
+          <t>How can I get married in Polish as a foreigner?</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://dord.dolnyslask.pl/</t>
+          <t>https://powroty.gov.pl/-/slub-z-cudzoziemcem-w-polsce</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Welcome to the website of the Lower Silesian Road Traffic Center. Select the city you are interested in for more information about a particular DORD branch.
-You can sign up for the Exam online, in which case click the button at the top of the page.</t>
+          <t>According to Polish law, marriage can be entered into by persons of legal age who are not married, are not related to each other in a straight line and are not siblings , are not related to each other in a straight line and are not in an adoption relationship . EXCEPTION! If the woman is a minor, but has reached the age of 16, or the persons are related to each other - they can get married if they get permission from the court. In addition, if a person is affected by mental illness or mental retardation - they can get married if they get court approval. Persons who are completely incapacitated cannot marry.</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://flowapps.pl/blog/jak-wymienic-ukrainskie-prawo-jazdy-na-polskie/</t>
+          <t>https://www.gov.pl/web/gov/wez-slub-cywilny</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Home - Blog - Tips - How to exchange a Ukrainian driver's license for a Polish one?
-Created by Piotr | Mar 4, 2025 | Advice | 0 comments
-If you are a citizen of Ukraine and reside in Poland, you are surely wondering how the issue of exchanging a Ukrainian driver's license for a Polish one. Thanks to the introduction of temporary European Union regulations, the process has been simplified. According to the Regulation of the European Parliament and of the Council (EU) of 2022, a Ukrainian driver's license is recognized on the territory of the European Union for persons under temporary protection, without the need to provide translations or an international driver's license.
-But... if you intend to work as a cab driver, or perform transportation services, you MUST HAVE a POLISH DRIVING LICENSE - this is a non-negotiable requirement. At the outset, it is important to mention that if you are afraid of this paperwork, we stand behind you - and Flow Apps offers full support and assistance in the process of legalization of residence and work for foreigners. In this article we take a closer look at what the process of exchanging a Ukrainian driver's license for a Polish one looks like.
-In recent months, there have been many questions about the exchange of driver's licenses for citizens of countries outside the European Union, particularly from Ukraine and Belarus. Drivers from these countries constitute an important group of employees, especially in the international transport sector for Polish transport companies. In connection with the end of temporary regulations related to the conflict in Ukraine and the introduction of the requirement to have a Polish driver's license for those providing paid transportation services (e.g. cabs, transportation in applications up to 9 people - such as Uber, Bolt, FreeNow, Bliq, among others), it is worth recalling the key rules on the exchange of driver's licenses for drivers from third countries.</t>
+          <t>If you have decided on a civil wedding - go to the registry office . There you will make the so-called assurance that there are no circumstances excluding the marriage and set the date of the wedding. You can also decide whether the wedding will be held in the office or outside, for example, in the open air. Below you will find only general information - ask the head of the USC for details. Expand the text Who can get married You can get married if: you are of legal age, you are not married, you are not related to each other in a straight line and you are not siblings , you are not related to each other in a straight line , you are not in an adoption relationship . If the woman is a minor, but has reached the age of 16 - she can get married if she gets permission from the court. If the persons are related to each other - they can get married if they get permission from the court. If a person is affected by mental illness or mental retardation - they can get married if they get court approval. Persons who are completely incapacitated cannot marry.</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://karta-pobytu.pl/baza-wiedzy/wymiana-zagranicznego-prawa-jazdy-na-polskie/</t>
+          <t>http://bip.brpo.gov.pl/pl/content/rpo-cudzoziemiec-malzenstwo-zaswiadczenie-problemy-mswia</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Are you considering exchanging your foreign driver's license for a Polish one? This may be necessary if you plan to settle in Poland and drive. Don't worry, our step-by-step guide will make the process surprisingly simple! In the article, we'll discuss the exchange procedure, required documents, details about different countries and useful information for foreigners. Start your adventure on Polish roads with confidence!
-Replacing a foreign driver's license with a Polish one may be necessary for those who intend to live and drive in Poland. The process may seem complicated, but with this guide you will learn how to go through it step by step. The following sections of the article will discuss the exchange procedure, the documents needed to apply for an exchange, the specifics of exchanging driver's licenses from different countries, and information for foreigners about the process.
-Note that the procedures may vary depending on your individual situation and the country from which the foreign driver's license originated. It is advisable to seek professional assistance from a law firm to ensure that the process goes smoothly and in accordance with current regulations.
-The process of exchanging a driver's license involves replacing a foreign driving permit with a Polish equivalent. The exchange is necessary for those who intend to live and drive in Poland permanently. General rules for the exchange include meeting formal requirements: reporting to the relevant communications department, submitting the required documents and paying the relevant fees.
-The procedure for exchanging a foreign driver's license for a Polish one consists of several steps. First, you need to report to the communications department responsible for your place of residence. Then, you need to submit the required documents, such as a foreign driver's license, a passport, as well as a certificate of registration. In some cases, it may also be necessary to provide a translation of the driver's license into Polish. Once all the formalities have been completed, the office will issue a decision to replace the driver's license, and then hand over the new document.</t>
+          <t>Problems with the certificate required for marriage to a foreigner. Replies of the Ministry of Internal Affairs and Administration Some registry offices do not accept certificates of a foreigner on the possibility to marry according to the law of his country and issued in it - if they do not contain the data of the other person who is to conclude the marriage It is not clear from Polish law that such a certificate must contain the data of the other nupturient</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>What are the rules for registering a foreign vehicle in Lower Silesia?</t>
+          <t>What are the requirements for family reunification visas in Polsky?</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://www.powiatwroclawski.pl/wydzial-komunikacji.html</t>
+          <t>https://www.gov.pl/attachment/59d481b9-ee0d-449a-b03f-9f0b8f114669</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Homepage
-Starostwo
-Departments / Offices</t>
+          <t>Temporary residence permit to reunite with ... Parent has a visa/temporary residence - Department of Foreigners Affairs Temporary residence permit for family members of citizens ...</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://mubi.pl/poradniki/rejestracja-samochodu-z-zagranicy/</t>
+          <t>https://www.mos.cudzoziemcy.gov.pl/informacje/zwiazek-mal</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Consent
-Details
-[#IABV2SETTINGS#]
-About cookies
-We use cookies to make our comparison engine work properly (essential cookies) and to provide you with personalized offers and services (functional, analytical and marketing cookies).</t>
+          <t>Temporary residence permit for the purpose of family reunification Select an area of interest or explore the full information regarding the permit The migration rules ensure that certain sponsors who are third-country nationals or stateless persons can exercise their right to family reunification, including:</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://bip.um.wroc.pl/attachments/download/152367</t>
+          <t>https://www.gov.pl/web/mswia/warunki-wjazdu-i-pobytu-cudzoziemcow-w-polsce</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Consent
-Details
-[#IABV2SETTINGS#]
-About cookies
-We use cookies to make our comparison engine work properly (essential cookies) and to provide you with personalized offers and services (functional, analytical and marketing cookies).</t>
+          <t>a valid long-term visa or a valid residence permit issued by Polish authorities; a document confirming possession of health insurance within the meaning of the Act of August 27, 2004. on health care services financed from public funds, or possession of travel medical insurance with a minimum insurance amount of 30,000 euros, valid for the period of the foreigner's planned stay in the territory of the Republic of Poland, covering all expenses that may arise during the stay in this territory due to the need to travel back for medical reasons, the need for urgent medical assistance, emergency hospital treatment or death, in which the insurer undertakes to cover the costs of medical services provided to the insured directly to the entity providing such services, on the basis of a bill issued by this entity - in the case of entry on a long-term visa. Information from the Minister of Foreign Affairs on insurers and insurances meeting these conditions can be found here: https://www.gov.pl/web/dyplomacja/wizy; The requirement to have medical insurance, as mentioned above, can be considered fulfilled if the foreigner has adequate insurance in connection with his or her professional situation; financial resources sufficient to cover the costs of the intended stay and the return trip to the country of origin or residence, or the costs of transit to a third country that will grant entry, or a document confirming the possibility of obtaining such funds in accordance with the law</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>How can I apply for Polish citizenship in Lower Silesia?</t>
+          <t>Can I have dual citizenship in Polish?</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://dudkowiak.pl/prawo-imigracyjne/jak-uzyskac-polskie-obywatelstwo/</t>
+          <t>https://bip.brpo.gov.pl/pl/content/rpo-podwojne-obywatelstwo-paszport-wyjazd-sg-odpowiedz</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Investor Zone
-Return
-Invest in Poland
-Return
-Invest in Poland
-Control of foreign investments in Poland
-IT outsourcing - a guide
-Company registration
-Return
-Company registration
-Limited partnership
-General partnership
-Civil partnership
-Representative office in Poland
-Branch office in Poland
-Subsidiary/target company
-Finished companies (shelf companies, shelf companies)
-Opening a bank account
-Limited liability company
-Joint Stock Company
-Labor law
-Return
-Labor law
-Remote work
-How to hire an employee in Poland?
-How much does it cost to hire an employee?
-Tax calculator
-Termination of employment contract
-Employee benefits
-Whistleblowers
-Employment contract template
-Working time
-Trade unions
-Employee Capital Plans (PPK).
-HR / Employment agency
-Legal proceedings
-Return
-Legal proceedings
-Maritime law
-Insurance law
-Arbitration
-Administrative penalties
-Tax law
-Return
-Tax law
-Corporate income tax (CIT)
-Guide to VAT
-Registration for VAT purposes
-VAT refund
-Capital gains tax
-Withholding tax (WHT)
-WHT Opinion
-Tax on dividends
-Tax Establishment in Poland (PE)
-Transfer Pricing
-MDR tax schemes
-Tax strategy
-Tax on civil law transactions (PCC)
-Real estate tax
-Tax Interpretations and Binding Rate Information
-Advance Pricing Agreements (APAs)
-General anti-avoidance clause (GAAR)
-The clause against tax avoidance (SAAR)
-Tax exemption for US army suppliers in Poland
-What is the Polish Family Foundation?
-Anti-dumping duty - how to avoid it?
-Debt collection
-Return
-Debt collection
-Court orders/payment orders
-Securing claims/claims
-Enforcement of foreign judgments
-Enforcement proceedings
-Rate of interest on late payment
-Bankruptcy and restructuring
-Limitation period
-Contract law
-Return
-Contract law
-B2B contract
-Franchise
-Real estate purchase
-Return
-Purchase of real estate
-Buying an apartment
-Buying a house
-Purchase of agricultural land
-Property Due Diligence
-Real estate register
-Mortgage
-Real estate purchase and taxes
-Purchase of real estate by a foreigner
-Lease of real estate
-Construction law
-Trademark
-Fintech
-Return
-Fintech
-MiCA implementation in Poland
-Lending institutions in Poland
-CASP license in Poland
-Small payment institution
-Electronic money institution
-VASP license in Poland | Cryptocurrency license.
-B2B loans/credit
-AML/CFT
-Corporate law
-Return
-Corporate law
-Share capital in a limited liability company.
-Management of the company
-Liability of the board of directors of a limited liability company for liabilities
-Representation in a limited liability company.
-Supervision in the company - Supervisory Board
-Proxy
-Shareholders' meeting
-Recapitalization of the company
-NBP reporting
-Taxation of the company
-Accounting in the company
-UBO/final beneficial owner
-Conversion into a joint stock company
-Liquidation of the company
-Foundation registration
-M&amp;A (mergers and acquisitions)
-Return
-M&amp;A (mergers and acquisitions)
-NDA agreements in Poland
-Concentration control
-Due Diligence
-Taxation of share transactions
-Acquisition of shares in a company
-Sale of shares in the company
-Regulated activities
-Return
-Regulated activities
-MIAA license for weapons and military products - a guide
-Regulation of CBD in Poland and the EU
-Mining law - mining licenses
-Gambling law
-Electromobility
-Environmental law
-Return
-Environmental law
-Protection of water and land
-Production of chemicals
-Gas Emission Reduction and Energy Efficiency
-Waste law
-Greenwashing
-CBAM
-Air Pollution Control
-Criminal law
-Return
-Criminal law
-Money laundering - what it is and what the penalties are
-European arrest warrant (EAW)
-Criminal liability of collective entities for prohibited acts
-Blocking of a bank account
-Defamation
-Cybercrime and bank fraud
-Antitrust/competition law
-Return
-Antitrust law/competition law
-Unfair competition
-Consumer protection
-Payment terms (delays)
-Advertising law
-Immigration law
-Return
-Immigration law
-Employment of UK citizens
-Temporary residence permit
-How to get a visa to Poland
-Polish citizenship for investment
-Permit to work in Poland
-Confirmation of Polish citizenship
-How to obtain Polish citizenship?
-Buying a car in Poland
-Employment of foreigners in Poland
-Inheritance law
-Return
-Inheritance law
-Statutory inheritance
-Testamentary inheritance
-Inheritance tax
-Inheritance of real estate
-Copyright
-Return
-Invest in Poland
-Return
-Invest in Poland
-Control of foreign investments in Poland
-IT outsourcing - a guide
-Return
-Invest in Poland</t>
+          <t>You have two citizenships - you must show your Polish passport when leaving Poland. Response from the Border Guard The Border Guard refuses Polish citizens with dual citizenship to cross the border to leave Poland on the basis of another country's passport Meanwhile, the regulations grant the right to have a passport, not an obligation. An adult citizen of the Republic of Poland residing in Poland is only obliged to have an identity card</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://www.lexmotion.eu/blog/requirements-for-polish-passport/</t>
+          <t>https://www.prawo.pl/prawo/podwojne-obywatelstwo-kiedy-mozliwe,523539.html</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Before applying for a Polish passport, you must first confirm your Polish citizenship. In this article, you will learn about the conditions and criteria that need to be met to obtain a Polish passport and enjoy its benefits.
-In today's globalized world, the ability to move freely and pursue personal development has become increasingly important.
-A Polish passport grants visa-free entry to 176 out of over 195 countries worldwide, making it one of the most valuable travel documents available.</t>
+          <t>Sebastian M., who was detained in Dubai and holds Polish and German citizenship, is no exception. In an increasingly globalizing world, two or even more passports in each suitcase are being legally held by more and more people, although not all countries look upon this favorably. "Dual citizenship serves as both an insurance policy and a method of opening up new opportunities. Having a second passport is also a plan B in case your country introduces some strange, unacceptable legislation, or the government is unstable," argues Andrew Henderson of Austin-based Nomad Capitalist , which specializes in off shore investments and tax optimization. However, dual citizenship is not always easy - eight European Japanese have sued to allow them to hold dual citizenship by choice . However, the Tokyo High Court, in a Sept. 28 ruling, dismissed their claims and ruled that it is constitutional to automatically lose Japanese citizenship if they voluntarily acquire another. "Dual citizenship can cause a conflict in rights and duties between countries, as well as between the individual and the state," the Japanese Supreme Court judges argue in their reasoning. Many people of Japanese descent live in the US, Brazil, Peru, Western European countries, and the Philippines, for example. The Japanese diaspora around the world numbers up to approx. 4 million people. If for some reason they are entitled to dual citizenship, they face the dilemma of which to choose. The Ministry of Justice in Tokyo reminds us that under laws in effect since 1985, Japan only allows dual citizenship for those younger than 22. When ending that age, one must decide - whether to stay with Japanese citizenship or choose foreign citizenship. This is what well-known tennis player Naomi Osaka did in 2019, surrendering her US passport. The appropriate statement to this effect must be made to officials in the Islands, and abroad at the consulate or embassy of the Land of the Cherry Blossom. On the other hand, those who obtained dual citizenship after their twentieth birthday have two years from that point to choose which passport they want to pocket. Japan is no exception - India, China and the United Arab Emirates are also on the list of countries automatically stripping their citizenship from those who acquire another. The citizenship of the Land of the Cherry Blossom is also among the hardest to acquire, even for those with Japanese roots or who work in Japan. "It's a complicated path, and we mainly focus on applications from Koreans who have been employed here for many years and have relatives here," stresses Ikuko Maekawa, a lawyer with an office in Osaka.</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://migrant.wsc.mazowieckie.pl/pl/procedury/nadanie-obywatelstwa-polskiego</t>
+          <t>https://powroty.gov.pl/czy-obywatel-polski-z-podwojnym-obywatelstwem-moze-w-polsce-poslugiwac-sie-amerykanskimi-dokumentami-jako-obywatel-jakiego-kraju-bedzie-tra-24074</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Go to main menu
-Skip to content
-Availability
-Home page
-Procedures</t>
+          <t>Can a Polish citizen with dual citizenship use American documents in Poland? As a citizen of which country will be treated after returning from emigration? Can a Polish citizen with dual citizenship use American documents in Poland? As a citizen of which country will he be treated upon his return? The legal provisions governing Polish citizenship are contained in the Constitution of the Republic of Poland and in the Act of April 2, 2009 on Polish citizenship . Polish law does not prohibit Polish citizens from obtaining foreign citizenship, whether by birth or through the process of naturalization, however, Polish authorities only recognize the Polish citizenship of such a person.</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>What are the language requirements for obtaining citizenship in Lower Silesia?</t>
+          <t>How to report a temporary stay in Poland?</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://www.migrant.info.pl/pl/uznanie-za-obywatela</t>
+          <t>https://www.gov.pl/web/gov/zamelduj-sie-na-pobyt-staly-lub-czasowy-dluzszy-niz-3-miesiace</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-We would like to draw your attention to the fact that the information provided on this website is not a source of law. We assure you that we have made every effort to comply with the applicable regulations. However, please note that this site is for informational purposes only, and the information on this site cannot be used as a basis in disputes with government authorities. If in doubt, we recommend that you contact the body conducting the administrative proceedings in a given case and familiarize yourself with the provisions of the law that may have a decisive impact on its resolution. We also invite you to contact the migrant.info hotline we run - +48 22 490 20 44
-We would like to draw your attention to the fact that the information provided on this website is not a source of law. We assure you that we have made every effort to comply with applicable regulations. However, please note that this site is for informational purposes only, and the information on this site cannot be used as a basis in disputes with government authorities. If in doubt, we recommend that you contact the body conducting the administrative proceedings in a given case and familiarize yourself with the provisions of the law that may have a decisive impact on its resolution. We also invite you to contact the migrant.info hotline we run - +48 22 490 20 44</t>
+          <t>Register for permanent or temporary residence longer than 3 months Are you changing your place of residence? Or are you returning from abroad and don't have a registration in Poland? Remember to register. You can do it online or at the municipality office. If you are a Polish citizen and your child was born in Poland - the head of the civil registry office that prepared the birth certificate will register your child ex officio.</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://www.dsw.edu.pl/strefa-studenta/aktualne-informacje-dla-studentow</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00210</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Dear Sirs,
-From November 20 to 28, 2024, electronic enrollment for elective (specialty) education modules through the USOSWeb system for Students of the following majors will start:
-Geodesy and Cartography,
-Computer Science,</t>
+          <t>The procedure for obtaining a temporary residence and work permit, i.e. a unified permit, is advantageous because all the formalities legalizing a foreigner's stay and employment take place under a single administrative procedure - the foreigner does not have to apply separately for a residence permit , and the employer - for a work permit. The provincial governor, who has granted a uniform permit for temporary residence and work in the territory of Poland, issues a residence card to the foreigner ex officio. The residence card, during the period in which it is valid, confirms the identity of the foreigner and entitles him, together with a travel document, to repeatedly cross the border without the need to obtain a visa.</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>http://www.przysiegly-niderlandzki-miw.pl/Blog%20Posts/jak-zostac-tlumaczem.html</t>
+          <t>https://www.gov.pl/web/uw-warminsko-mazurski/cudzoziemcy---zezwolenia-na-pobyt-czasowy-na-terytorium-rp</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-To become a sworn Dutch translator, one must first of all be fluent in Dutch and Polish, but not only that. Since 2006, one must also additionally pass a two-stage exam at the Ministry of Justice, consisting of a written and an oral part. Unfortunately, knowledge of both languages and passing the exam does not yet entitle an interpreter to perform debt translations.
-The profession of a sworn translator is a profession of public trust, so under the Law on the Profession of Sworn Translators, candidates are required to:
-Have Polish citizenship or citizenship of another EU or EFTA country, or citizenship of a country covered by the "reciprocity principle."
-Have not been convicted of intentional, fiscal or economic crimes,</t>
+          <t>Detailed information can be found on the website of the Office for Foreigners in the Case Service Module at the following link: https://www.mos.cudzoziemcy.gov.pl/potrzebuje-informacji/pobyt-czas https://mos.cudzoziemcy.gov.pl/potrzebuje-informacji/szczegolne-okol</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Can I have dual citizenship in Lower Silesia?</t>
+          <t>What should be included in my employment contract in Polish?</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://kancelariadso.pl/aktualnosci/czy-mozna-miec-podwojne-obywatelstwo</t>
+          <t>https://zielonalinia.gov.pl/-/umowa-o-prace-co-powinna-zawierac</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Start
-right-arrow_777</t>
+          <t>The employer should sign an employment contract with you before you start working. According to the Labor Code, Article 29 §2 The employment contract shall be concluded in writing. If the employment contract is not concluded in writing, the employer shall, before allowing the employee to work, confirm to the employee in writing the arrangements as to the parties to the contract, the type of contract and its terms. It is impermissible to provide work without a signed contract or the terms and conditions established in writing.</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://czasopisma.uwm.edu.pl/index.php/sp/article/download/8796/7205/33470</t>
+          <t>https://zielonalinia.gov.pl/obowiazki-pracownika-i-pracodawcy-33373</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Start
-right-arrow_777</t>
+          <t>Familiarizing employees who take up work with the scope of their duties, the way they perform their work and their basic rights, ensuring safe and hygienic working conditions and systematic training of employees in this regard, facilitating employees to improve their professional qualifications,</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>https://www.radiowroclaw.pl/articles/view/137528/J-Protasiewicz-o-wnioskach-cudzoziemcow-Przez-2-lata-nie-zdazylibysmy-ich-obsluzyc-Trzeba-to-usprawnic</t>
+          <t>https://zielonalinia.gov.pl/umowa-o-prace-33374</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-Jacek Protasiewicz, Deputy Governor of Lower Silesia, was a guest at Radio Wroclaw's Talk of the Day.
-I wanted to start by saying that government administration is a place where you have not worked before, but you corrected that 34 years ago you were the spokesman for the Lower Silesian governor.
-Yes. That was my first job, one during the romantic period when Poland was transitioning from an authoritarian, communist system to one that was democratic. Tadeusz Mazowiecki's government appointed the first governors, well, not PZPR governors, and the spokesman for the first governor, Mr. Jaroslaw Muszynski, was me. Also working in the same corridor, on the opposite side of the corridor was my office.</t>
+          <t>for a probationary period of up to three months to test the employee's qualifications, minimum wage , prohibition of termination and termination of employment in special cases,</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Can I open a bank account in Lower Silesia as a foreigner?</t>
+          <t>What are the health care and social security premiums for foreigners in Poland?</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://www.pkobp.pl/klient-indywidualny/konta/jak-otworzyc-konto-osobiste?srsltid=AfmBOor8QFuVbvFvLpCHmHjqVDV1jKiWzNgsRO1j59LoGr1zEca6kGvy</t>
+          <t>https://www.biznes.gov.pl/pl/portal/00291</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Open a bank account online and choose how to sign the contract - confirm your identity online for a selfie or receive a courier delivery with the contract
-Download and launch the IKO app, then choose Open an account on selfie
-Enter your contact information, give the appropriate consents, and select your account type and payment card. Take photos of your ID and face, check the accuracy of your data, indicate your home address, accept the statements and submit the application
-Sign the agreement online and use your account!Some features e.g. e-Office will require additional proof of identity at the branch1
-How to quickly transfer your account to PKO Bank Polski?</t>
+          <t>Who can do business in Poland Even if you do not have Polish citizenship, you have the right to undertake and carry out business activities in Poland. In addition, you may offer or provide temporary services or establish a branch or representative office of your company in Poland.</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://www.kontomaniak.pl/poradniki/konto-dla-obcokrajowca-gdzie-zalozyc</t>
+          <t>https://www.gov.pl/web/zdrowie/finansowanie-leczenia-cudzoziemcow-w-polsce</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Statistics show that there are about 2.5 million foreigners living in Poland in 2024. This is a sizable number of people, many of whom work or study in our country. They also have bank accounts. In this article, we'll look at what should characterize an account for a foreigner, how to open one and where to do it.
-Table of contents:
-How to open an account for a foreigner?
-Account for a foreigner - documents
-Is it possible to open an account for a foreigner without a residence card?</t>
+          <t>If you are insured in EU/EFTA member states If your stay is temporary you can receive only necessary medical care. You will receive the following benefits on the same basis as those insured in Poland: provision of orthopedic items and auxiliary aids,</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>https://polskabezgotowkowa.pl/dla-ciebie/artykuly/jak-zalozyc-konto-w-banku-bez-polskiego-obywatelstwa/</t>
+          <t>https://www.gov.pl/web/rodzina/pomoc-spoleczna-dla-cudzoziemcow-na-jakie-wsparcie-w-polsce-moga-liczyc</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Consent
-Details
-[#IABV2SETTINGS#]
-About
-Necessary 6 Necessary cookies help make a website usable by enabling basic functions like page navigation and access to secure areas of the website. The website cannot function properly without these cookies.Cookiebot1Learn more about this providerCookieConsentStores the user's cookie consent state for the current domainMaximum Storage Duration: 1 yearType: HTTP CookieCriteo1Learn more about this provideroptoutIdentifies if the visitor has deselected any cookies, trackers or other audience targeting tools.Maximum Storage Duration: SessionType: HTTP CookieGoogle2Learn more about this providerSome of the data collected by this provider is for the purposes of personalization and measuring advertising effectiveness.ar_debugChecks whether a technical debugger-cookie is present. Maximum Storage Duration: 30 daysType: HTTP Cookietest_cookieUsed to check if the user's browser supports cookies.Maximum Storage Duration: 1 dayType: HTTP CookieID51Learn more about this providergdprDetermines whether the visitor has accepted the cookie consent box. This ensures that the cookie consent box will not be presented again upon re-entry.  Maximum Storage Duration: SessionType: HTTP CookieNativo1Learn more about this provideropt_outUsed to detect if the visitor has accepted the marketing category in the cookie banner. This cookie is necessary for GDPR-compliance of the website.  Maximum Storage Duration: 1 yearType: HTTP Cookie</t>
+          <t>Social assistance for foreigners. What support in Poland can they count on? Foreigners in Poland are not left on their own. What social assistance support can they count on? What conditions must they meet? We explain in a practical guide. Persons entitled to social assistance - in addition to those with Polish citizenship - are also foreigners who are domiciled and reside in Poland, among others:</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>What documents are needed to apply for a loan or mortgage in Lower Silesia?</t>
+          <t>What are the requirements for permanent residence in Poland?</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://www.kingaburcan.pl/doradca-kredytowy-wroclaw/kredyt-hipoteczny-wroclaw/</t>
+          <t>https://powroty.gov.pl/zezwolenie-na-pobyt-staly-10025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Consent
-Details
-[#IABV2SETTINGS#]
-About
-Necessary 6 Necessary cookies help make a website usable by enabling basic functions like page navigation and access to secure areas of the website. The website cannot function properly without these cookies.Google3Learn more about this providerSome of the data collected by this provider is for the purposes of personalization and measuring advertising effectiveness.test_cookiePendingMaximum Storage Duration: 1 dayType: HTTP Cookierc::aThis cookie is used to distinguish between humans and bots. This is beneficial for the website, in order to make valid reports on the use of their website.Maximum Storage Duration: PersistentType: HTML Local Storagerc::cThis cookie is used to distinguish between humans and bots. Maximum Storage Duration: SessionType: HTML Local StorageUsercentrics GmbH2Learn more about this providerucDataStores the user's cookie consent state for the current domainMaximum Storage Duration: PersistentType: HTML Local StorageucStringNecessary for the correct implementation of the websites Consent Management Platform (CMP)Maximum Storage Duration: PersistentType: HTML Local Storagewww.kingaburcan.pl1CookieConsentStores the user's cookie consent state for the current domainMaximum Storage Duration: 1 yearType: HTTP Cookie</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>https://erif.pl/poradnik-konsumenta/jak-dostac-kredyt-na-mieszkanie-jakie-warunki-nalezy-spelnic/</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Home Consumer Guide How to get a loan for an apartment? What conditions must be met?
-For most of us, the realization of the dream of our own house or apartment involves taking out a mortgage. This long-term commitment is quite a risk for banks, so they put a number of conditions for the future borrower to meet before granting the loan. From our article you will learn how to take out a mortgage and how to increase your chances of getting a positive credit decision.
-A mortgage is a financial obligation that is secured by a mortgage. This means that if you stop paying the installments, the bank can sell the mortgaged property (through a bailiff) to recover the borrowed money in this way.
-It is worth knowing that the lender does not gain such powers automatically. A mortgage is a limited right to a thing, and it is established by the owner of the property, making an entry in the land records after the loan has already been granted. Deletion of the entry takes place after repayment of the obligation.The mortgage encumbers the property, not the owner. Thus, you can both sell an apartment with a mortgage and buy it. The new owner will then be obliged to repay the obligation. Before buying a property, check the land records to ensure that the property is not burdened with debt.</t>
-        </is>
-      </c>
+          <t>Legalization of residence in Poland of the spouse/partner of a foreigner Information according to the legal status as of: 2024-09-04 The spouse of a Polish citizen who is not a citizen of one of the EEA countries or Switzerland, i.e. a citizen of a so-called third country, may apply for a permanent residence permit.</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://grupaang.pl/kredyty-i-pozyczki/pozyczka-hipoteczna/</t>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/cudzoziemcy-18053962/art-195</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Consent
-Details
-[#IABV2SETTINGS#]
-About cookies
-Essential 12 Essential cookies are absolutely necessary for the proper functioning of the website. These cookies anonymously provide the basic functionality and security of the website.Google7Learn more about this providerSome of the data collected by this provider is used to personalize and measure the effectiveness of advertising.test_cookiePendingMaximum retention period: 1 dayName: HTTP_GRECAPTCHAThis cookie is used to distinguish between humans and bots. This is beneficial for the website, in order to make valid reports on the use of their website.Maximum retention period: 180 daysName: HTTP_grecaptchaThis cookie is used to distinguish between humans and bots. This is beneficial for the website, in order to make valid reports on the use of their website.Maximum retention period: PermanentName: Local HTMLrc storage::aThis cookie is used to distinguish between humans and bots. This is beneficial for the website, in order to make valid reports on the use of their website.Maximum retention period: PermanentName: Local HTMLrc storage::bThis cookie is used to distinguish between humans and bots. Maximum retention period: SessionName: Local HTMLrc storage::cThis cookie is used to distinguish between humans and bots. Maximum retention period: SessionalName: Local HTMLrc storage::fThis cookie is used to distinguish between humans and bots. Maximum retention period: PersistentName: Local HTML storageangfinanse.pl1wpEmojiSettingsSupportsThis cookie is part of a bundle of cookies which serve the purpose of content delivery and presentation. The cookies keep the correct state of font, blog/picture sliders, color themes and other website settings.Maximum retention period: SessionalName: Local HTMLconsent.cookiebot.comporownywarkahipoteczna.angfinanse.pl2CookieConsent [x2]Stores the user's cookie consent state for the current domainMaximum retention period: 1 yearName: HTTP cookieporownarkahipoteczna.angfinanse.pl1tokenUsed to make live streaming of video content more efficient.Maximum retention period: PersistentName: Local storage HTMLwww.un.org.pl1PHPSESSIDPreserves user session state across page requests.Maximum retention period: SessionBenchmark: HTTP cookie</t>
+          <t>Article 195 - - Foreigners. If you want to access all related documents, log in to LEX Not yet using LEX programs? Order test access " How can a foreigner with a permanent residence permit be employed?</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>How can I report a crime as a foreigner in Lower Silesia?</t>
+          <t>What are the rules for registering a foreign vehicle in Polish?</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://przybysz.duw.pl/cudzoziemcy-pobyt/zezwolenia-na-pobyt-staly/</t>
+          <t>https://samorzad.gov.pl/web/powiat-jasielski/rejestracja-pojazdu-sprowadzonego-z-zagranicy</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Who makes the request?
-When should I/we submit the application?
-How do I submit an application?
-What documents do I need to submit?
-What are the fees?</t>
+          <t>Registration of a used vehicle imported from abroad I. Application II. Attachments to the application: 1) Proof of ownership of the vehicle, and if the vehicle is entrusted by a foreign legal or natural person to a Polish entity - a document confirming the entrustment of the vehicle, 2) Statement of the date of importation of the vehicle from the territory of a member state of the European Union, if attached to the proof of ownership of the vehicle, 3) Registration certificate, if the vehicle was registered - a party to the agreement on the European Economic Area, instead of the registration certificate it is allowed to present another document stating the registration of the vehicle, issued by the authority competent for the registration of vehicles in that country), 4) Registration plates, if the vehicle was registered; in the case of a vehicle imported from abroad without license plates or the necessity of returning these plates to the registration authority of the country from which the vehicle was imported, the vehicle owner, instead of license plates, shall attach a statement that the vehicle was imported from abroad without license plates or a statement of the necessity of returning these plates to the registration authority of the country from which the vehicle was imported; the statement may be made on the application for registration, including on the back thereof, 5) Proof of import clearance, if the vehicle was imported from the territory of a country that is not a member state of the European Union and is registered for the first time. If the vehicle is sold by a vehicle trader, this document may be replaced by an endorsement on the invoice specifying the date and number of the proof of import clearance and the name of the authority that cleared the vehicle. 6) A document confirming the payment of excise duty in the national territory or a document confirming that there is no obligation to pay excise duty in the national territory or a certificate stating exemption from excise duty, within the meaning of the provisions on excise duty, if a passenger car, a vehicle of the type "automobile other", a sub-type "quadricycle" or a sub-type "light quadricycle" , truck , sub-type "van", "van/pod", "truck/passenger", "off-road", "multipurpose" or "van" or special car , was imported from the territory of a member state of the European Union and is registered for the first time.</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>https://www.podlaski.strazgraniczna.pl/pod/cudzoziemcy/konsekwencje-nielegalne</t>
+          <t>https://powroty.gov.pl/-/rejestracja-samochodu-sprowadzonego-z-zagranicy-krok-po-kroku</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Go to main menu
-Skip to content
-Skip to search engine
-Site map
-Homepage</t>
+          <t>In Poland, buying a car imported from abroad is a very popular form of acquiring a two-wheeler. Statistics show that such cars arrive in our country about a million a year. There is also no shortage of cars bought by Poles abroad, used there and brought back to Poland after their return. According to Art.71(1) of the Road Traffic Law: the document stating that a motor vehicle has been admitted to traffic is a registration certificate or a temporary permit. Therefore, any car that has not yet been registered in Poland must be registered .</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>https://kancelaria-adwokacka-warszawa.pl/deportacja/</t>
+          <t>https://powroty.gov.pl/procedura-rejestracji-9531</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>If the foreigner does not have any residence title in Poland, such as a visa or residence permit, his stay here is illegal and he faces deportation from Poland. The decision on the obligation to return is issued by the competent Border Guard Commander. The deportation decision may specify a deadline for voluntary return of 15 to 30 days. However, in cases where it is likely that the foreigner will not voluntarily leave Poland or is required by reasons of defense or national security, the deadline for voluntary return is not specified, and the execution of the decision is immediate. This means that the deportation of the immigrant takes place immediately regardless of the fact that he has the right to appeal against such a decision.
-It should be remembered that the Law on Foreigners also provides for the possibility of deportation of a foreigner legally residing in Poland. The reasons for deportation in such a case are, among others, performance of work without a proper permit, undertaking economic activity in violation of the law, being sentenced to imprisonment in the Republic of Poland by a final judgment, the authority's recognition that the foreigner's further stay poses a threat to public order and security even without a criminal conviction, or the authority's determination that the purpose and conditions of the foreigner's stay in Poland are inconsistent with those declared.
-However, the law provides for situations when, even in the case of the occurrence of grounds for deportation in relation to a foreigner, a decision obliging the foreigner to return is not issued.
-In the decision on the obligation to return, the authority may establish a period of prohibition of re-entry. Consequently, a foreigner who leaves Poland as a result of such a deportation decision may not immediately return to Poland. When a deportation decision imposes a period of prohibition on the foreigner's re-entry into Poland, it is possible for the law firm to apply for the revocation of such a prohibition and thus allow the foreigner to return to Poland more quickly.
-It is also possible to avoid the re-entry ban altogether.</t>
+          <t>Registration of a used vehicle imported from a country that is not a member of the European Union Registration of a used vehicle imported from a country that is not a member of the European Union Information according to the legal status as of: 2024-09-06</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Where can I find free legal assistance in Lower Silesia?</t>
+          <t>Can I drive in Poland on a foreign driver's license?</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://www.kancelariakrs.pl/ile-kosztuje-porada-prawna-u-adwokata-prawnika-radcy-prawnego-notariusza/</t>
+          <t>http://bip.brpo.gov.pl/pl/content/rpo-polskie-prawo-jazdy-utrata-ue-kara-mc</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Home " Blog " How much does it cost for legal advice from an attorney, lawyer, solicitor, notary?
-Katarzyna Knapek
-Legal audit, Frankovichs, Residence of foreigners, Legal assistance for companies, Civil law, Law for the construction industry, Business law, Criminal law, Real estate law, Labor law, Family law, Contract law, Law in debt collection, Law in public procurement, RODO, Consumer bankruptcy, Trademarks
-February 26, 2021
-Where is free legal advice possible? How much does it cost to get legal help from a lawyer, legal advisor or notary? We check the price lists of legal services, explain what the cost of legal advice in our and other law firms in Katowice depends on.</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
+          <t>Lose your Polish driver's license and get one somewhere in the EU? In Poland you will be punished for its absence. RPO's intervention A citizen who loses his driver's license in Poland and obtains one in another EU country is treated in Poland as a person driving a vehicle without authorization, and is punished for this This also restricts the constitutional freedom of movement within the territory of the Republic of Poland</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>https://powroty.gov.pl/prawo-jazdy-5285</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Information according to the legal status as of: 2024-09-06 Any person who has a driver's license issued abroad and has lived in Poland for at least 185 days must exchange it for a Polish driver's license. A foreign driver's license ceases to be valid 6 months after permanent or temporary residence in Poland. This also applies to driving licenses issued in the UK after December 31, 2020. However, the obligation to replace the driver's license does not apply to those who have:</t>
+        </is>
+      </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>https://www.wroclaw.pl/dla-mieszkanca/pomoc-dla-cudzoziemcow-wroclaw</t>
+          <t>https://www.gov.pl/attachment/c7c9da8f-f437-4626-88a0-72e9d704a922</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Consent
-Details
-Ads settings
-About cookies
-Collect data on your geographic location with an accuracy of up to a few meters</t>
+          <t>Information according to the legal status as of: 2024-09-06 Any person who has a driver's license issued abroad and has lived in Poland for at least 185 days must exchange it for a Polish driver's license. A foreign driver's license ceases to be valid 6 months after permanent or temporary residence in Poland. This also applies to driving licenses issued in the UK after December 31, 2020. However, the obligation to replace the driver's license does not apply to those who have:</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>What should I do if I am arrested or fined in Lower Silesia?</t>
+          <t>What documents are needed to apply for a loan or mortgage in Polsky?</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://gazetawroclawska.pl/tydzien-z-nowymi-mandatami-za-nami-na-dolnym-slasku-posypaly-sie-wysokie-kary/ar/c1-15987509</t>
+          <t>https://www.gov.pl/web/mieszkanie-dla-ciebie/program-pierwsze-mieszkanie</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>This website is using a security service to protect itself from online attacks. The action you just performed triggered the security solution. There are several actions that could trigger this block including submitting a certain word or phrase, a SQL command or malformed data.
-You can email the site owner to let them know you were blocked. Please include what you were doing when this page came up and the Cloudflare Ray ID found at the bottom of this page.
-Cloudflare Ray ID: 92f550bbbb4deec7
--
-      Your IP:
-      Click to reveal
-83.27.101.111
--
-Performance &amp; security by Cloudflare</t>
+          <t>10 Reasons to Choose First Housing If you're ready to buy your first apartment or single-family home - from July 1, 2023, you can take advantage of the secure 2% loan, or mortgage subsidy system. If you plan to do so in the next few years - from the same moment you can save for their purchase in a Housing Account. The regulations that allow you to apply for a 2% safe loan and open a Housing Account came into effect on July 1, 2023.</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>https://tvn24.pl/wroclaw/172</t>
+          <t>https://www.gov.pl/web/mieszkanie-dla-ciebie/pytania-i-odpowiedzi</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>TVN24 live
-TVN24 BiS live
-TVN24 in Ukrainian
-TVN24NewsWorldPolandBusinessMeteoPremiumSportsHealthTechnologyCulture and styleInteresting news.
-FactsSee FactsFacts After FactsFacts About the WorldFacts After NoonFacts People.</t>
+          <t>The answers to the following questions do not constitute an interpretation of the law with respect to individual cases, but a general interpretation of the provisions of the Act of May 26, 2023 on State Aid to Housing Savings, amending the Act of October 1, 2021 on Family Housing Credit and 2% Safe Credit. The final assessment of the fulfillment of the conditions of the "First Housing" program rests with the participating bank. If a positive verification of meeting the statutory criteria is made, it is the bank that will decide on the possibility of granting a 2% safe loan and establishing a Housing Account. The Ministry of Development and Technology is not involved in this process. The parties to the contract for a 2% safe loan or the operation of a Housing Account are the borrower/saver and the bank granting the loan or operating the Account. The Ministry of Development and Technology is not a party to such an agreement, and is not involved in the process of granting a loan or opening an Account. Therefore, any questions on the provisions of the agreement should be addressed to the bank with which such an agreement was concluded. There is no limitation on the price per square meter of a residential unit. Also in the case of a combination of a 2% secured loan and a guarantee of the borrower's own contribution.</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://www.facebook.com/PolicjaKG/?locale=gl_ES</t>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/kredyt-hipoteczny-oraz-nadzor-nad-posrednikami-kredytu-18594631/roz-2</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>1m</t>
+          <t>Chapter 2 - Obligations of the lender, mortgage intermediary and agent before entering into a mortgage contract - Mortgage credit and supervision of mortgage intermediaries and agents. Obligations of the creditor, mortgage intermediary and agent prior to the conclusion of a mortgage credit agreement The creditor, mortgage intermediary and agent may provide to the consumer, prior to the conclusion of a mortgage credit agreement, on a durable medium, additional data other than those specified in Article 11, paragraph 1, including the information form referred to in Article 11, paragraph 2.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>How can I get a work permit as a non-EU citizen in Poland?</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/ou1611</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Fill out and send an electronic application at praca.gov.pl. You will sign it with a qualified signature or trusted profile. Permit type A or B for work of a foreigner on the territory of Poland Are you an entrepreneur, you have a company in Poland and you want to hire a foreigner from outside the EU, EEA or Switzerland? You must first obtain a type A or B work permit for him or her. Read how these permits differ and how to obtain them.</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00295</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Citizens of countries outside the European Union, the European Economic Area or Switzerland, may work in Poland provided that: the entrepreneur who wants to employ them obtains an appropriate work permit for them, or the foreigner has a uniform permit for temporary residence and work.</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/004330</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>A foreigner who is a citizen of a country outside the European Union , the European Economic Area or Switzerland may legally work in Poland, provided that he or she meets the following conditions together: legally resides in the territory of Poland, i.e. has the appropriate residence documents if he or she is not exempt from the obligation to have a work permit, then: he obtains a temporary residence and work permit or the employer obtains for him a work permit, a seasonal work permit or submits a statement on entrusting work to a foreigner his residence documents allow him to perform work his work is performed under the conditions and in the position specified in the work permit, statement on entrusting work or temporary residence and work permit .</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>How can I report an employer who does not pay my salary in Polish?</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00199</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>The subject of a complaint filed with the State Labor Inspectorate may be violations of labor laws by the posting employer, including health and safety regulations and regulations concerning the legality of employment. In the case of a posting of up to 12 months, an employee posted to work in Poland may file a complaint if the employer fails to provide him with conditions of employment concerning: the norms and dimensions of working time and daily and weekly rest periods</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00197</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Employees posted to Poland are entitled to the remuneration specified in their contracts. As a rule, failure to pay wages to an employee posted in the territory of Poland is the responsibility of the posting employer. Failure to pay remuneration to a delegated employee constitutes an offense against the rights of persons performing gainful employment and is punishable by a fine from PLN 1,000 to PLN 30,000.</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/finanse/stop-nielegalnemu-zatrudnieniu-i-placeniu-pod-stolem</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Stop illegal employment and under-the-table payments The Polish Deal is also a measure to curb "black market" work and the payment of wages "under the table." Starting next year, the tax and contribution consequences of these titles will be borne by dishonest employers, not their employees.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>What rights do I have as a tenant in Polsky?</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/kodeks-cywilny-16785996/ks-3-tyt-17-dz-1</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>A contract for the lease of real estate or premises for a period longer than one year should be concluded in writing. If this form is not observed, the contract shall be deemed to have been concluded for an indefinite period. If during the term of the lease the thing requires repairs, which are borne by the lessor, and without which the thing is not fit for the agreed use, the lessee may set a reasonable time limit for the lessor to perform the repairs. After ineffective expiration of the set deadline, the lessee may make the necessary repairs at the expense of the lessor. If a third party asserts claims against the lessee regarding the leased thing, the lessee shall immediately notify the lessor.</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>https://www.prawo.pl/biznes/najemca-obowiazany-jest-zwrocic-rzecz-w-stanie-niepogorszonym,151236.html</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>The tenant is to repair the damage when he moves out of the apartment The tenant is to repair the damage when he moves out of the apartment According to the Civil Code, the tenant is responsible for such consequences of using the premises that exceed the consequences of normal use. On the other hand, however, the law obliges the tenant, for example, to repair the walls and floors of the leased premises. Rightly, many people see the possibility of renting an apartment as a good way to secure a monthly income. However, relations between landlord and tenant do not always run smoothly. Difficulties arise especially when it is necessary to account for the cost of repairs associated with the use of a house or apartment. It is important to remember that the provisions of the Civil Code do not close the issue, and it is necessary to reach for detailed regulations. According to them, most minor repairs are charged to the tenant.</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/kodeks-cywilny-16785996/art-673</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Article 673 - - Civil Code. If you want to access all related documents, log in to LEX Not yet using LEX programs? Order trial access " What is the situation of tenants of commercial premises in housing cooperatives during the coronavirus?</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>How to get health insurance in Poland?</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>http://pacjent.gov.pl/archiwum/2021/jak-ubezpieczyc-sie-dobrowolnie</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>If you live in Poland and are not covered by universal health insurance, nor are you entitled to benefits, you can take advantage of voluntary insurance Apply to the provincial branch of the National Health Fund (NFZ) competent for your place of residence or to one of the branch's delegations. You will find a list of current addresses of provincial branches on the NFZ website. Fill out an application for voluntary health insurance coverage. You can print the application and fill it out at home or on the spot at the branch. You will find a sample document at the bottom of the page.</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>https://www.nfz.gov.pl/dla-pacjenta/ubezpieczenia-w-nfz/</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Insurance in the NFZ eWUŚ How to insure yourself voluntarily Oncology package opens in a new tab Provision of medical devices The Constitution guarantees you the right to health care, but you may not always be entitled to free, i.e. publicly financed, health care services. Law of August 27, 2004 on publicly funded health care benefits ;</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>https://www.nfz.gov.pl/dla-pacjenta/ubezpieczenia-w-nfz/jak-sie-ubezpieczyc-dobrowolnie/</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Insurance in the NFZ eWUŚ How to insure yourself voluntarily Oncology package opens in a new tab Provision of medical devices A contract with the NFZ voluntarily entitles you to: all publicly funded health care services on the same terms as for other insured persons under the public health care system,</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>How can I register a company in Polish?</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00120</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Check if you can run a business in Poland You can run a sole proprietorship on your own if you are an adult, because only then you are fully responsible for your actions and have full decision-making capacity. Minors who want to run their own business will have to use their legal representatives in many situations. Most often these will be parents.</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00119</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>The Polish Classification of Business Activities is a systematization of business activities used in public statistics, records and accounting. As of January 1, 2025, the new Polish Classification of Activities - PKD 2025, which replaced the previous one - PKD 2007, is in force. PKD 2025 has been adapted to changes made in the classification of the European Union , current market, technological and social realities. It includes activities that have emerged in the economy in recent years, related, for example, to the digital economy, the circular economy or the bioeconomy. Descriptions of traditional industries have also been clarified.</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00172</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>There are various definitions of business in the laws governing business. When conducting business, it is important to take into account whether a particular activity constitutes a business within the meaning of the relevant regulations. For income tax purposes, a business activity is a profit-making activity: involving the exploration, prospecting and extraction of minerals from deposits</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>How to apply for a residence card in Poland?</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/uw-podlaski/zasady-skladania-wnioskow-i-odbioru-kart-pobytu</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Create an account in the Case Service Module - mos.cudzoziemcy.gov.pl - fill out the application for temporary residence or permanent residence electronically, print it out with a barcode, sign it in person and, together with the required documents, send it to the Office via a postal operator or submit it - with a receipt - at the Customer Service Point of the Podlaskie Voivodship Office in Bialystok at 3 Mickiewicza Street . Applications completed electronically at the MOS will be directly forwarded for processing upon receipt at the Office, and the foreigner will receive a written summons to appear in person for fingerprinting on the specified date and time. Priority will also be given to long-term resident permit applications completed on paper, sent by mail or submitted to the Authority's Service Desk, due to the lack of an electronic filing service at the MOS. An instructional video on how to fill out an application for a temporary residence permit using the electronic form at the MOS can be found at: https://www.youtube.com/watch?v=CQwDzLXejjo&amp;t=8s Fill out the application for temporary residence or permanent residence in traditional form and send it, together with the required documents, to the Office through the postal operator or submit it - against receipt - at the Customer Service Center at the Office. Applications filled out traditionally, outside the MOS, will be forwarded for processing no earlier than 6 months from the date of their receipt at the Office. After this date, the foreigner will receive a written summons to appear in person for fingerprinting on the specified date and time. Submission of applications for replacement of a residence card, issuance of a Polish travel document for a foreigner, collection of a residence card and a Polish travel document for a foreigner is carried out without taking a ticket from a ticket machine: at the Foreigners' Service Room - post No. 5 Monday 7:15 - 17:45 Tuesday, Thursday, Friday 8:00 - 15:00</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00210</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>The procedure for obtaining a temporary residence and work permit, i.e. a unified permit, is advantageous because all the formalities legalizing a foreigner's stay and employment take place under a single administrative procedure - the foreigner does not have to apply separately for a residence permit , and the employer - for a work permit. The provincial governor, who has granted a uniform permit for temporary residence and work in the territory of Poland, issues a residence card to the foreigner ex officio. The residence card, during the period in which it is valid, confirms the identity of the foreigner and entitles him, together with a travel document, to repeatedly cross the border without the need to obtain a visa.</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00210#2</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>The procedure for obtaining a temporary residence and work permit, i.e. a unified permit, is advantageous because all the formalities legalizing a foreigner's stay and employment take place under a single administrative procedure - the foreigner does not have to apply separately for a residence permit , and the employer - for a work permit. The provincial governor, who has granted a uniform permit for temporary residence and work in the territory of Poland, issues a residence card to the foreigner ex officio. The residence card, during the period in which it is valid, confirms the identity of the foreigner and entitles him, together with a travel document, to repeatedly cross the border without the need to obtain a visa.</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>How to get a driver's license in Poland?</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/gov/uzyskaj-prawo-jazdy</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Do you want to obtain a driver's license? Do you have a driver's license and want another category? Check out how to do it. Expand the text Who can get a driver's license can be obtained by anyone who has lived in Poland for at least 185 days and: wants to get a driver's license for the first time - if he or she is the right age, already has a driver's license and wants to get another category - if he or she is the right age. Check the minimum age requirement for each category of driver's license. You can apply by proxy. Find out at the office how to do this. A driver's license can be obtained by anyone who has lived in Poland for at least 185 days and:</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/infrastruktura/jak-uzyskac-prawo-jazdy-</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Do you want to obtain a driver's license? Or do you already have one and want to get a permit for the next category? Find out how the whole process looks like - from submitting an application, through the course and exam, to receiving the document. If you want to apply for a driver's license online, click on the "Over the Internet" link. any Polish citizen who wants to get a driver's license for the first time - if he or she is of the age required for the category. Check the minimum required age for each category of driver's license, any adult Polish citizen who already has a driver's license and wants to obtain a permit for another category ,</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/gov/kategorie-prawa-jazdy</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Want to get a driver's license? Find out what vehicles you can drive in each category and how old you need to be to pass the test to drive them. Expand text Driver's license categories Category name What vehicles you can drive How old do you have to be to get a driver's license AM moped quadricycle light combination of vehicles - the above vehicles combined with a trailer - only in Poland 14 years A1 motorcycle with an engine displacement of up to 125 cm3, power of up to 11 kW and a power to kerb weight ratio of up to 0.1 kW/kg three-wheeled motorcycle with a power of up to 15 kW AM category vehicles combination of vehicles - the above vehicles combined with a trailer - only in Poland 16 years A2 motorcycle that meets all of the following conditions: power up to 35 kW power to kerb weight ratio up to 0.2 kW/kg it must not be the result of modifications to the vehicle, whose power exceeds twice the power of that motorcycle three-wheeled motorcycle with a power of up to 15 kW vehicles of category AM combination of vehicles - the above vehicles combined with a trailer - only in Poland 18 years A any motorcycle vehicle of category AM combination of vehicles - the above vehicles combined with a trailer - only in Poland 20 years - if you have already for at least 2 years A2 license 24 years - if you have not for at least 2 years A2 license B1 quadricycle vehicle of category AM 16 years B motor vehicle with a maximum permissible weight of up to 3,5 t , with the exception of a bus and motorcycle a combination of vehicles - the above vehicle combined with a light trailer a vehicle from category AM a combination of vehicles - consisting of a motor vehicle with a gross vehicle weight of up to 3.5 t and a trailer. However, the total permissible weight of the entire team can not exceed 3500 kg, if you pass an additional practical test and have an additional entry in your driver's license - a team of vehicles - composed of a motor vehicle with a gross vehicle weight of up to 3.5 t and a trailer. However, the total permissible weight of the entire team must not exceed 4250 kg agricultural tractor - only in Poland a slow-moving vehicle - only in Poland a team of vehicles consisting of an agricultural tractor and a light trailer - only in Poland a team of vehicles consisting of a slow-moving vehicle and a light trailer - only in Poland if you have a category B driver's license for at least 3 years - a motorcycle with an engine capacity of up to 125 cm3, power up to 11 kW and a power to kerb weight ratio up to 0.1 kW/kg - only in Poland 18 years B+E a vehicle combination of a vehicle from category B and a trailer with a maximum permissible weight up to 3.5 t a vehicle combination of an agricultural tractor and a trailer or trailers - only in Poland a vehicle combination of a slow-moving vehicle and a trailer or trailers - only in Poland 18 years C a motor vehicle with a maximum permissible weight over 3,5 t, except for a bus a combination of vehicles - the above vehicle and a light trailer a vehicle from category AM an agricultural tractor - only in Poland a slow-moving vehicle - only in Poland a combination of vehicles consisting of an agricultural tractor and a light trailer - only in Poland a combination of vehicles consisting of a slow-moving vehicle and a light trailer - only in Poland 21 years C1 a motor vehicle with a permissible total weight over 3.5 t to 7.5 t, except for a bus a combination of vehicles - the above vehicle and a light trailer a vehicle from category AM an agricultural tractor - only in Poland, a slow-moving vehicle - only in Poland a combination of vehicles consisting of an agricultural tractor and a light trailer - only in Poland a combination of vehicles consisting of a slow-moving vehicle and a light trailer - only in Poland 18 years C1+E a combination of vehicles with a maximum permissible weight of up to 12 tons, which consists of: a vehicle that pulls - vehicles from category C1 a trailer a vehicle combination consisting of an agricultural tractor and a trailer or trailers - only in Poland a vehicle combination consisting of a slow-moving vehicle and a trailer or trailers - only in Poland 18 years C+E a vehicle combination consisting of a vehicle from category C and a trailer, a combination of vehicles made up of an agricultural tractor and a trailer or trailers - only in Poland a combination of vehicles made up of a slow-moving vehicle and a trailer or trailers - only in Poland 21 years D bus a combination of vehicles made up of a bus and a light trailer a vehicle from category AM an agricultural tractor - only in Poland a slow-moving vehicle - only in Poland a combination of vehicles made up of an agricultural tractor and a light trailer - only in Poland a combination of vehicles made up of a slow-moving vehicle and a light trailer - only in Poland 24 years D1 a bus designed by design to carry up to 17 persons including the driver, with a length of up to 8 m a combination of vehicles consisting of the vehicle referred to above, and a light trailer a vehicle of category AM an agricultural tractor - only in Poland a slow-moving vehicle - only in Poland a vehicle combination consisting of an agricultural tractor and a light trailer - only in Poland a vehicle combination consisting of a slow-moving vehicle and a light trailer - only in Poland 21 years D1+E combination of vehicles composed of a vehicle of category D1 and a trailer combination of vehicles composed of an agricultural tractor and a trailer or trailers - only in Poland combination of vehicles composed of a slow-moving vehicle and a trailer or trailers - only in Poland 21 years D+E combination of vehicles composed of a vehicle of category D and a trailer trailers a combination of vehicles consisting of an agricultural tractor and a trailer or trailers - only in Poland a combination of vehicles consisting of a slow-moving vehicle and a trailer or trailers - only in Poland 24 years T agricultural tractor a slow-moving vehicle a combination of vehicles consisting of an agricultural tractor and a trailer or trailers a combination of vehicles consisting of a slow-moving vehicle and a trailer or trailers a vehicle of category AM 16 years Tram 21 years You can start the course and take the driving test for a specific category even before you reach the age indicated above - but not earlier than 3 months before. Therefore, apply for a driver's license no earlier than 3 months before this age. The information in this sheet does not apply to driving vehicles of the Armed Forces of the Republic of Poland, the State Fire Service, the Police, the Border Guard Service. A combination of vehicles - the above vehicles combined with a trailer - only in Poland</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Are there any legal restrictions on renting an apartment by a foreigner in Poland?</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/attachment/727a25ae-43bf-461a-8d45-c35e444e5c64</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Draft No. 950 - on amending the Law on foreigners and ... On amending the Law on granting protection to foreigners on ...</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/ou209</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Obtain a permit for the acquisition of real estate by a foreigner Are you a foreigner from outside the European Union, Switzerland, Norway, Iceland and Liechtenstein and intend to acquire real estate in Poland? You'll need to obtain a permit from the minister. Check out how to do it. What you should know and who can use the service</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>https://www.malopolska.uw.gov.pl/doc/pouczenie_dla_cudzoziemcow.doc</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Obtain a permit for the acquisition of real estate by a foreigner Are you a foreigner from outside the European Union, Switzerland, Norway, Iceland and Liechtenstein and intend to acquire real estate in Poland? You'll need to obtain a permit from the minister. Check out how to do it. What you should know and who can use the service</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>How can I report a crime as a foreigner in Polsky?</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>https://bip.brpo.gov.pl/pl/content/rpo-cudzoziemcy-przestepstwa-zawiadomienia-kgp-odpowiedz</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>The issue of foreigners who do not know Polish language filing oral reports of crime. Response from KGP Deputy RPO Stanislaw Trociuk addressed Police Chief Insp. Marek Boron regarding the provision of an interpreter to foreigners who report a crime to their detriment The obligation to call an interpreter occurs when the person being interrogated does not speak Polish, even if the interrogating police officer knows the foreign language spoken by the person. Importantly, the interrogated persons do not bear the cost of the interpreter's participation, the KGP explains</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>https://lublin.policja.gov.pl/llu/prewencja/dla-cudzoziemcow/64544,Jak-zlozyc-zawiadomienie-o-popelnionym-przestepstwie.html</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>How to report a crime If you have been victimized by a crime - , or have directly witnessed such an event MAKE A NOTICE OF CRIME COMPLETION To do this, the best way is to go to the nearest police station or prosecution unit. You can give notice orally or in writing. To report orally is to tell the police officer/prosecutor about the entire incident. After giving an oral notice, you may be immediately questioned as a witness. Both the notice and the interrogation will be recorded in a protocol, which will be filled out by the police officer/prosecutor. Finally, the protocol must be signed by you. If you wish to give notice in writing, leave the letter containing the information you would like to give to law enforcement at the police station or prosecutor's office, or send it by mail .</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>https://ksp.policja.gov.pl/download/168/25021/Jakpowinienpostepowapolicjantwykonujacyczynnoscizudzialemcudzoziemca.pdf</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>How to report a crime If you have been victimized by a crime - , or have directly witnessed such an event MAKE A NOTICE OF CRIME COMPLETION To do this, the best way is to go to the nearest police station or prosecution unit. You can give notice orally or in writing. To report orally is to tell the police officer/prosecutor about the entire incident. After giving an oral notice, you may be immediately questioned as a witness. Both the notice and the interrogation will be recorded in a protocol, which will be filled out by the police officer/prosecutor. Finally, the protocol must be signed by you. If you wish to give notice in writing, leave the letter containing the information you would like to give to law enforcement at the police station or prosecutor's office, or send it by mail .</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>How to enroll a child in school in Poland?</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>https://www.prawo.pl/oswiata/jak-zapisac-dziecko-do-szkoly-jakie-dokumenty-potrzebne-czym-jest-rejonizacja-szkol-podstawowych,374408.html</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Criteria for recruitment to elementary schools - decided by the law and local government regulations Criteria for recruitment to elementary schools - decided by the law and local government regulations The legal basis for recruitment to elementary schools are the provisions of the Education Law and the provisions of the Regulation of the Minister of Education on the conduct of recruitment and supplementary proceedings to public kindergartens, schools, institutions and centers.</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>https://powroty.gov.pl/-/wracamy-do-polskiej-szkoly</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Certificates, certificates, certificates, or what documents you will need Returning from emigration is certainly a logistical challenge. Formalities, documents, packing of accumulated belongings, and still the awareness of all the formalities waiting for you upon your return. In the midst of all these issues, there are still children - their preparation: mental, but also practical matters such as education. There is also the question: what documents of the child will be required in a Polish school? The standard documents required from the local school are certificates, if there are any in the country's school system, or a certificate issued by the management of the school where the child studied. In addition, if the child also attended a Polish school, the so-called Saturday school - certificates from consecutively completed classes will be needed. All these documents, relating to the child's education abroad, will allow to confirm the fulfillment of compulsory education and will provide information on the grades obtained by the child. On the basis of the mentioned documents, the school director will be able to decide which class the child should be admitted to.</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>https://powroty.gov.pl/na-jakich-warunkach-moje-dzieci-moga-zostac-przyjete-do-polskiej-szkoly-12138</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Under what conditions can my children be admitted to a Polish school? We are returning with our children from Iceland after 3 years of stay. Will we have problems enrolling them in school once the school year starts? They speak very little Polish and we are afraid that they will end up in classes with much younger children. Any student arriving/returning from abroad is admitted to school in Poland on the basis of:</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>What are the conditions for obtaining Polish citizenship?</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>https://powroty.gov.pl/nabycie-obywatelstwa-polskiego-10000</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Information according to the legal status as of: 2024-09-11 The issues of acquiring Polish citizenship and losing it are regulated by the Act of April 2, 2009 on Polish citizenship. 1. birth from parents, at least one of whom has Polish citizenship - the rule of blood/Ius Sanguinis</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>https://archiwum.mswia.gov.pl/pl/bezpieczenstwo/obywatelstwo-i-repatri/cudzoziemcy/10169,SPOSOBY-NABYCIA-OBYWATELSTWA-POLSKIEGO.html</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>The issues of acquiring Polish citizenship and losing it are regulated by the Act of April 2, 2009 on Polish citizenship . The Act contains two basic principles concerning Polish citizenship. The principle of continuity of Polish citizenship, expressed in Article 2 of the Act, guarantees the permanence of citizenship in time, starting from the moment of its acquisition, in accordance with the provisions in force at the time, regardless of changes to the legislation concerning citizenship. This means that persons who acquired Polish citizenship on the basis of old laws, subsequently repealed or amended, if they have not lost their Polish citizenship, retain it in accordance with the laws in effect on the date of acquisition. This principle is at the same time a directive to the competent public administration bodies in proceedings to confirm possession or loss of Polish citizenship. On the other hand, the principle of the exclusivity of Polish citizenship, introduced by the provision of Article 3 of the Law, is closely related to the problem of dual citizenship, as it creates a clear conflict directive in the event of its occurrence and allows for the removal of its adverse effects. The draft law adopts the principle of permissibility of multiple citizenships while maintaining the absolute priority of Polish citizenship. A Polish citizen may simultaneously hold Polish citizenship and citizenship of a foreign state, but even then he or she has the same rights and obligations towards the Republic of Poland as a person holding only Polish citizenship, i.e. he or she cannot invoke with legal effect towards the Polish authorities the foreign citizenship held simultaneously or the rights and obligations arising from it. Birth from parents, at least one of whom has Polish citizenship - Rule of blood/Ius Sanguinis</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/mswia/uzyskaj-polskie-obywatelstwo</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Confirmation of possession or loss of Polish citizenship Want to get Polish citizenship? Have you lost your Polish citizenship and want to regain it? Do you need official confirmation that you have Polish citizenship? Here you will find all the information you need. Apply to the President for Polish citizenship</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Do I need a work permit in Polsky?</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/uw-lodzki/kiedy-cudzoziemiec-nie-potrzebuje-zezwolenia-na-prace</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>When does a foreigner not need a work permit? A foreigner may work in the territory of Poland if: has refugee status granted in the Republic of Poland;</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/ou1611</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Fill out and send an electronic application at praca.gov.pl. You will sign it with a qualified signature or trusted profile. Permit type A or B for work of a foreigner on the territory of Poland Are you an entrepreneur, have a company in Poland and want to hire a foreigner from outside the EU, EEA or Switzerland? You must first obtain a type A or B work permit for him or her. Read how these permits differ and how to obtain them.</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>https://zielonalinia.gov.pl/-/cudzoziemcy-zwolnieni-z-obowiazku-posiadania-zezwolenia-na-prace-cz-1-</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>When we look for regulations defining foreigners who are authorized to perform work on the territory of Poland without a work permit, we reach for the Act of April 20, 2004 on employment promotion and labor market institutions and the Regulation of the Minister of Labor and Social Policy of April 21, 2015 on cases in which entrusting work to a foreigner on the territory of the Republic of Poland is permitted without a work permit. In addition, the Law of December 12, 2013 on foreigners is also useful. In the first part of this article, we will present the cases described in the Law on Employment Promotion and Labor Market Institutions. According to Article 87 (1) of the Law on Employment Promotion and Labor Market Institutions, a foreigner is entitled to work in the territory of Poland if, among other things: 1) has refugee status granted in the Republic of Poland;</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>What are the rules of family reunification in Poland?</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/attachment/59d481b9-ee0d-449a-b03f-9f0b8f114669</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Temporary residence permit to reunite with ... Temporary residence permit to reunite with ... Family reunification - Podlaskie Provincial Office in ...</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>https://www.mos.cudzoziemcy.gov.pl/informacje/zwiazek-mal</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Temporary residence permit for the purpose of family reunification - marriage recognized by the law of the Republic of Poland Select an issue of interest to you or learn more about the full information on the permit Migration regulations provide the opportunity to exercise the right to family reunification to certain members of the separated family who are third-country nationals or who are stateless, including:</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>https://mos.cudzoziemcy.gov.pl/informacje/maloletni-benef/wymogi</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Temporary residence permit for the purpose of family reunification - parent or guardian of an unaccompanied minor beneficiary of international protection Select an issue of interest to you or learn more about the full permit In order for a foreigner to obtain a temporary residence permit for the purpose of family reunification, it is necessary for him to meet the following requirements cumulatively:</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>How to rent an apartment in Poland legally?</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>https://www.prawo.pl/student/jak-bezpiecznie-wynajac-mieszkanie-bedac-studentem,520206.html</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>The rules for renting an apartment are governed by the Civil Code and the Law on the Protection of Tenants' Rights, Housing Resources of Municipalities and Amendments to the Civil Code . According to Article 659 of the Civil Code, by a lease agreement the lessor undertakes to give the lessee a thing to use for a definite or indefinite period of time, and the lessee undertakes to pay the lessor the agreed rent. Rent may be denominated in money or in benefits of another kind. A lease agreement for real estate or premises for a period longer than one year should be concluded in writing. If this form is not observed, the contract shall be deemed to have been concluded for an indefinite period. The indication of the term in the concluded agreement is of great importance in the context of determining the notice period. In this case, in accordance with Article 673 of the Civil Code, which includes the terms of termination of the lease, it is assumed that if the duration of the lease is not fixed, both the lessor and the lessee may terminate the lease by contractual terms, and in their absence by statutory terms.</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/kodeks-cywilny-16785996/ks-3-tyt-17-dz-1</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>A contract for the lease of real estate or premises for a period longer than one year should be concluded in writing. If this form is not observed, the contract shall be deemed to have been concluded for an indefinite period. If during the term of the lease the thing requires repairs, which are borne by the lessor, and without which the thing is not fit for the agreed use, the lessee may set a reasonable time limit for the lessor to perform the repairs. After ineffective expiration of the set deadline, the lessee may make the necessary repairs at the expense of the lessor. If a third party asserts claims against the lessee regarding the leased thing, the lessee shall immediately notify the lessor.</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/rozwoj-technologia/spoleczne-agencje-najmu3</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>A social rental agency is an entity that works with a municipality to mediate between rental housing owners and people whose income or living situation makes it difficult to rent an apartment under market conditions. to increase the housing supply for middle- and lower-income people, expanding the tools available to municipalities in implementing local housing policy to include a formula that can provide an alternative to municipal housing,</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>What should I do if I am arrested or fined in Polsky?</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>https://mazowiecka.policja.gov.pl/wsi/aktualnosci/78630,Areszt-za-niezaplacona-grzywne-Jak-i-kiedy.html</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Did you fail to accept a fine or pay a fine and think you'll get away with it? Nothing could be further from the truth. An unpaid fine results in a conversion to a jail term of a few days to as much as 6 months on the same case. How to protect yourself from this? How many days in jail for what amount of fine? This is what you will find out below. If a person refuses to accept a fine, the police send a request for punishment to the District Court. The court decides whether the person is guilty or innocent. In the case of established guilt in minor cases, a fine is adjudged, at the same time ruling - in case of non-payment - the conversion of the fine to arrest, counting one day of arrest from 50 zlotys to 1,500 zlotys fine. The total duration of detention can not exceed 6 months in the same case. Such a judgment is sent to the convicted person. There is a note in it about the amount of the fine, the account number and the deadline for payment after the judgment becomes final. If the person downplays the letter received and does not pay the fine, the case again returns to court, where the fine is converted to a custodial sentence. When converting a fine into a substitute prison sentence, the court assumes that one day of imprisonment equals two daily rates of fine. Thus, if there are 100 daily rates of fine of 20 zlotys each to be paid, the court will impose 50 days of alternate punishment. If the person does not appear in custody and continues to fail to pay the adjudicated fine then the court will issue a Detention and Bring Order along with an order to initiate a nationwide search and send it to the Police. According to the Law on Police, we carry out the orders of the court and the prosecutor's office. Uniformed officers have a month's time to detain and bring such a person into custody, otherwise the court may issue a letter of appointment for such a person, which can be published on websites, in the press and in the media.</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>https://sip.lex.pl/procedury/ukaranie-kara-porzadkowa-grzywny-lub-pozbawienia-wolnosci-za-naruszenie-powagi-sadu-1610615575</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Stefanski Ryszard A., Punishment with a penalty of a fine or imprisonment for violation of the solemnity of a court Punishment with a penalty of a fine or imprisonment for violation of the solemnity of a court Punishment with a penalty of a fine or imprisonment for violation of the solemnity of a court Punishment with a penalty of a fine or imprisonment for violation of the solemnity of a court</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/kodeks-karny-wykonawczy-16798687/CZ-.sz</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Special part - Fine - Executive Penal Code. The session on ordering the execution of a substitute sentence of imprisonment shall be attended by the prosecutor, the convicted person and his defense counsel, and when the convicted person is under supervision - also by the court professional probation officer, a trustworthy person or a representative of an association, institution or social organization referred to in Article 73 § 1 of the Penal Code. When granting a convict conditional early release from serving the remainder of the sentence of imprisonment, the penitentiary court may, if there are grounds for assuming that the convict will pay the fine voluntarily, suspend the previously ordered execution of the alternative sentence of imprisonment, at the same time applying Article 49; in that case, the period of installment of the fine shall run from the date of the decision on conditional early release.</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>How can I exchange my driver's license for a Polish one in Polskie?</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/gov/wymien-zagraniczne-prawo-jazdy-na-polskie</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>European Union member countries: Austria / Austria Belgium Belgium Bulgaria / Bulgaria Croatia / Croatia Cyprus Czech Republic / Czechia Denmark / Denmark Estonia Finland / Finland France / France Greece / Greece Spain / Spain Netherlands / Netherlands Ireland / Ireland Lithuania / Lithuania Luxembourg / Luxembourg Latvia / Latvia / Malta / Malta Germany / Germany Portugal / Portugal Romania / Romania Slovakia / Slovakia Slovenia / Slovenia Sweden / Sweden Hungary / Hungary / Hungary Italy / Italy Do you have a foreign driver's license and have lived in Poland for a minimum of 185 days? Exchange it for a Polish driver's license. Check out how to do it. If you have a valid driver's license from an EU country - you do not need to exchange it for a Polish driver's license. A driving license from an EU country is valid in Poland.</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>https://powroty.gov.pl/prawo-jazdy-5285</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Information according to the legal status as of: 2024-09-06 Any person who has a driver's license issued abroad and has lived in Poland for at least 185 days must exchange it for a Polish driver's license. A foreign driver's license ceases to be valid 6 months after permanent or temporary residence in Poland. This also applies to driving licenses issued in the UK after December 31, 2020. However, the obligation to replace the driver's license does not apply to those who have:</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/gov/wymien-prawo-jazdy</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Are you moving or changing your name and your driver's license is invalid? Replace it. Find out how to do it. Expand the text Who must replace Anyone who has changed: name or surname. Anyone whose: driver's license has become invalid, driving license category has become invalid. The matter can also be handled by proxy. Find out at the office how to do this. The matter can also be handled by proxy. Find out at the office how to do it.</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>What are the language requirements for obtaining citizenship in Polish?</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>https://archiwum.mswia.gov.pl/pl/bezpieczenstwo/obywatelstwo-i-repatri/cudzoziemcy/10169,SPOSOBY-NABYCIA-OBYWATELSTWA-POLSKIEGO.html</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>The issues of acquiring Polish citizenship and losing it are regulated by the Act of April 2, 2009 on Polish citizenship . The Act contains two basic principles concerning Polish citizenship. The principle of continuity of Polish citizenship, expressed in Article 2 of the Act, guarantees the permanence of citizenship in time, starting from the moment of its acquisition, in accordance with the provisions in force at the time, regardless of changes to the legislation concerning citizenship. This means that persons who acquired Polish citizenship on the basis of old laws, subsequently repealed or amended, if they did not lose their Polish citizenship, retain it in accordance with the laws in effect on the date of acquisition. This principle is at the same time a directive to the competent public administration bodies in proceedings to confirm possession or loss of Polish citizenship. On the other hand, the principle of the exclusivity of Polish citizenship, introduced by the provision of Article 3 of the Law, is closely related to the problem of dual citizenship, as it creates a clear conflict directive in the event of its occurrence and allows for the removal of its adverse effects. The draft law adopts the principle of permissibility of multiple citizenships while maintaining the absolute priority of Polish citizenship. A Polish citizen may simultaneously hold Polish citizenship and citizenship of a foreign state, but even then he or she has the same rights and obligations towards the Republic of Poland as a person holding only Polish citizenship, i.e. he or she cannot invoke with legal effect towards the Polish authorities the foreign citizenship held simultaneously or the rights and obligations arising from it. Birth from parents, at least one of whom has Polish citizenship - Rule of blood/Ius Sanguinis</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/mswia/uzyskaj-polskie-obywatelstwo</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Confirmation of possession or loss of Polish citizenship Want to get Polish citizenship? Have you lost your Polish citizenship and want to regain it? Do you need official confirmation that you have Polish citizenship? Here you will find all the information you need. Apply to the President for Polish citizenship</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/dolnoslaski-uw/uznanie-za-obywatela-polskiego</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Obtain Polish citizenship through an administrative decision issued by the Lower Silesian Governor. a foreigner residing continuously on the territory of the Republic of Poland for at least 3 years on the basis of a permanent residence permit, a residence permit for a long-term resident of the European Union or the right of permanent residence, who has a stable and regular source of income in the Republic of Poland and the legal title to occupy a dwelling, or a foreigner residing continuously on the territory of the Republic of Poland for at least 2 years on the basis of a permanent residence permit, a residence permit for a long-term resident of the European Union or the right of permanent residence, who: has been married for at least 3 years to a Polish citizen or has no citizenship, or</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>How to start a company in Poland as a foreigner?</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00806</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Who can do business in Poland Citizens of the European Union member states and the European Economic Area who want to do business in Poland can: set up their own sole proprietorship or any commercial company</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00806#2</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Who can do business in Poland Citizens of the European Union member states and the European Economic Area who want to do business in Poland can: set up their own sole proprietorship or any commercial company</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>https://www.biznes.gov.pl/pl/portal/00806#4</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Who can do business in Poland Citizens of the European Union member states and the European Economic Area who want to do business in Poland can: set up their own sole proprietorship or any commercial company</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>How can I get my rental deposit back in Polish?</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>https://sip.lex.pl/akty-prawne/dzu-dziennik-ustaw/ochrona-praw-lokatorow-mieszkaniowy-zasob-gminy-i-zmiana-kodeksu-16903658/art-6</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Article 6 - - Protection of tenants' rights, housing stock of the municipality and amendment of the Civil Code. If you want to access all related documents, log in to LEX Not yet using LEX programs? Order trial access " Should the amount of the deposit be returned to the tenant's bank account if the tenant is in arrears on the lease of the premises, including rent arrears?</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>https://powroty.gov.pl/kaucja-8433</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Information according to the legal status as of: 2023-10-11 A refundable deposit/deposit , which you receive when you return the keys to your apartment, is usually applicable to a rental agreement in the UK. It is usually equal to three months' rent, although there are also cases of one or two months' rent. The deposit, which we paid when signing the contract, is much easier to recover in full when renting an apartment privately. It is slightly more difficult to recover 100 percent of the amount paid if you rent an apartment or room through an agency. The landlord or the agency have the right to deduct from the deposit the costs of damage done by the tenants or unpaid bills. In many cases it even comes to counting every defect that is not included in the protocol usually attached to the rental agreement.</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>https://www.prawo.pl/prawo/problemy-z-najmem-okazjonalnym,513120.html</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Occasional lease - unpaid bills can be covered by security deposit Occasional lease - unpaid bills can be covered by security deposit The occasional lease seems to be a suitable solution for many parties to such contracts. It appears as a safe solution especially for landlords, who can count on the tenant to voluntarily leave the occupied premises in case of problems, since he should indicate another address where he can move out of the leased apartment.</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Where can I find free legal assistance in Polsky?</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/gov/skorzystaj-z-darmowej-pomocy-prawnej</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Take advantage of free legal, civic advice and mediation Do you need help from a lawyer, civic advisor, mediator? Are you in a difficult situation in life, for example, you need help with installment debt, repayment of "momentary" loans, you have housing problems, you have encountered difficulties finding a job, you do not know what office to go to for help, you have other problems related to everyday life issues? Go for civic advice.</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/nieodplatna-pomoc</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Free legal aid, civic advice and mediation are provided at about 1,500 points in Poland - in every county People with special needs Learn more</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>https://www.gov.pl/web/nieodplatna-pomoc/dyzury-specjalistyczne</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>At the beginning of 2022, on-call services with a specific specialization were launched at selected points of free legal aid and free civic counseling. A specialization is an indication of the area of law or other subject matter to which the advice applies or the group of people entitled to assistance. Specialized on-call points are separate on-call points with an additionally specified specialization. The introduction of specialized points makes it possible to offer and use the knowledge and experience of free assistance lawyers and citizen advisors with an indication of their specialization. The beneficiary of assistance can find a specialist in the field that interests him. An analysis of the topics of advice carried out in previous years has made it possible to identify the areas of law most relevant to the beneficiaries of free assistance. These include assistance to families raising children with disabilities and assistance to victims of violence against women and children. Points with such specializations have been established alongside those specializing in inheritance law, franking credits, insurance, taxation or consumer bankruptcy.</t>
         </is>
       </c>
     </row>

</xml_diff>